<commit_message>
Added Story001 & Story002 Analysis and Conception to RapportDeTravail, Updated MCD and MLD, Added SQL script for country and places creation (cH only)
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Mise à jour du repository git, envoi de la planification initiale</t>
+  </si>
+  <si>
+    <t>Analyse des modifications à apportées à l'API pour répondre aux critères du cahier des charges. J'ai pu remarquer que le cahier des charges intègre de nouvelles informations aux activités tel que le lieu et pays de réalisation de l'activité.</t>
+  </si>
+  <si>
+    <t>Conception</t>
+  </si>
+  <si>
+    <t>Je mets à jour le MCD et le MLD pour correspondre aux attentes du cahier des charges. J'ajoute ensuite au rapport de travail le nouveau MCD et le nouveau MLD</t>
+  </si>
+  <si>
+    <t>Je mets à jour le schéma de base de données à l'aide de MySQL Workbecnh. Je créer un script permettant d'insérer toutes les localités de suisse dans la base de données. J'ai trouvé un fichier contenant les localités sur le site admin.ch</t>
+  </si>
+  <si>
+    <t>J'enregistre le nouveau endpoint (Country) sur l'API, j'ai ensuite créer les méthodes permettant de sélectionner les pays et les localités de ceux-ci</t>
+  </si>
+  <si>
+    <t>Je me suis aperçu que le format de retour de l'API n'est pas tout à fait adapté quand beaucoup d'enregistrement sont envoyés.</t>
   </si>
 </sst>
 </file>
@@ -162,8 +180,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E24">
-  <autoFilter ref="A1:E24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E45">
+  <autoFilter ref="A1:E45"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -438,17 +456,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C26:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
@@ -582,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="1">
         <v>43592</v>
       </c>
@@ -609,6 +627,7 @@
       <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1">
@@ -623,59 +642,215 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
+    <row r="13" spans="1:8" ht="60">
+      <c r="A13" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B13">
+        <v>0.75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" ht="45">
+      <c r="A14" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="60">
+      <c r="A15" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="60">
+      <c r="A16" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
       <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="1"/>
-      <c r="D24" s="4"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1"/>
+      <c r="D45" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C24">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C45">
       <formula1>"Gestion, Analyse, Conception, Implémentation, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added formidable module, Added formidable middleware, Updated MLD with new way of handling files, Updated Activity creation method, Added Utiliy method do swap name of object property
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -2,20 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI_PHILIBERT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11085" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
-    <sheet name="Totaux" sheetId="3" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="17" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -90,16 +93,49 @@
     <t>Conception</t>
   </si>
   <si>
-    <t>Je mets à jour le MCD et le MLD pour correspondre aux attentes du cahier des charges. J'ajoute ensuite au rapport de travail le nouveau MCD et le nouveau MLD</t>
-  </si>
-  <si>
-    <t>Je mets à jour le schéma de base de données à l'aide de MySQL Workbecnh. Je créer un script permettant d'insérer toutes les localités de suisse dans la base de données. J'ai trouvé un fichier contenant les localités sur le site admin.ch</t>
-  </si>
-  <si>
     <t>J'enregistre le nouveau endpoint (Country) sur l'API, j'ai ensuite créer les méthodes permettant de sélectionner les pays et les localités de ceux-ci</t>
   </si>
   <si>
     <t>Je me suis aperçu que le format de retour de l'API n'est pas tout à fait adapté quand beaucoup d'enregistrement sont envoyés.</t>
+  </si>
+  <si>
+    <t>Étiquettes de lignes</t>
+  </si>
+  <si>
+    <t>Total général</t>
+  </si>
+  <si>
+    <t>Somme de Temps (h)</t>
+  </si>
+  <si>
+    <t>Je mets à jour le schéma de base de données à l'aide de MySQL Workbench. Je créer un script permettant d'insérer toutes les localités de suisse dans la base de données. J'ai trouvé un fichier contenant les localités sur le site admin.ch</t>
+  </si>
+  <si>
+    <t>Je mets à jour le MCD et le MLD pour correspondre aux attentes du cahier des charges. J'ajoute ensuite au rapport de travail le nouveau MCD et le nouveau MLD. J'ai également écris les tests sur le endpoint Country</t>
+  </si>
+  <si>
+    <t>Je me rends compte que la réponse représente une quantité d'information assez importante (actuellement 8'000 lignes), je pense que je pourrais diminuer la taille de la requête en ajoutant des filtres sur le nom de la commune par exemple</t>
+  </si>
+  <si>
+    <t>Test du enpoint créée hier (Country) avec les tests postman</t>
+  </si>
+  <si>
+    <t>Analyse des besoins du client lors de la création d'une activité avec un fichier GPX</t>
+  </si>
+  <si>
+    <t>Conception de la gestion des fichiers sur l'API. J'aimerai améliorer cette gestion de fichier car la solution actuelle ne permet pas la gestion de fichier volumineux. J'imagine plusieurs solutions pour palier à ce problème</t>
+  </si>
+  <si>
+    <t>Je crée le middleware de gestion des requêtes multipart. Cette fonctionnalitée est assez rapidement implémentée car j'avais déjà écrit d'autres middleware pour l'API précédament</t>
+  </si>
+  <si>
+    <t>Tests des modifications apportées sur le endpoint de création d'activités. J'effectue les tests avec des GPX fournit par Monsieur Glassey</t>
+  </si>
+  <si>
+    <t>Modification de la création d'activité dans le modèle d'activité pour prendre en compte les champs traité par le middleware Formidable. J'ai créer une méthode dans la classe d'utility pour me permettre de changer le nom des propriétés d'un objet, cela va m'être utile lorsque les paramètres d'une requête HTTP ne correspondent pas aux noms de champs dans la base de données</t>
+  </si>
+  <si>
+    <t>Je me suis rendu compte que les timestamps étaient décaler d'une heure, j'ai dabord cru que le problème vennait du format de timestmap que je fournissait en paramètre, mais le problème vennait en faite de la connection au serveur MySQL, je ne spécifait pas le timezone.</t>
   </si>
 </sst>
 </file>
@@ -143,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -155,6 +191,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -177,6 +218,1536 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[PHILIBERT_JournalDeBord.xlsx]Feuil1!Tableau croisé dynamique2</c:name>
+    <c:fmtId val="3"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Répartition type d'activité</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4B0F-416B-AF98-AA10F2CF9C7B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4B0F-416B-AF98-AA10F2CF9C7B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4B0F-416B-AF98-AA10F2CF9C7B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-4B0F-416B-AF98-AA10F2CF9C7B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Analyse</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Conception</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gestion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Implémentation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-4B0F-416B-AF98-AA10F2CF9C7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3438524</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="PHILIBERT Alexandre" refreshedDate="43594.61665891204" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="44">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Journal[[Date]:[Type]]"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Date" numFmtId="164">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-10T00:00:00"/>
+    </cacheField>
+    <cacheField name="Temps (h)" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="1.5"/>
+    </cacheField>
+    <cacheField name="Type" numFmtId="0">
+      <sharedItems containsBlank="1" count="5">
+        <s v="Gestion"/>
+        <s v="Analyse"/>
+        <s v="Conception"/>
+        <s v="Implémentation"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="44">
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="1.5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-07T00:00:00"/>
+    <n v="0.5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-05-08T00:00:00"/>
+    <n v="0.75"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-05-08T00:00:00"/>
+    <n v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-08T00:00:00"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2019-05-08T00:00:00"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2019-05-09T00:00:00"/>
+    <n v="0.5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2019-05-09T00:00:00"/>
+    <n v="0.5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-05-09T00:00:00"/>
+    <n v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-09T00:00:00"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2019-05-09T00:00:00"/>
+    <n v="1.5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2019-05-09T00:00:00"/>
+    <n v="1"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="4"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item h="1" x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Somme de Temps (h)" fld="1" baseField="0" baseItem="363412240"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,16 +2029,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C26:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="57.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -622,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>13</v>
@@ -660,7 +2231,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="45">
+    <row r="14" spans="1:8" ht="60">
       <c r="A14" s="1">
         <v>43593</v>
       </c>
@@ -671,7 +2242,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -686,7 +2257,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -701,40 +2272,104 @@
         <v>6</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
-      <c r="D18" s="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="105">
+      <c r="A17" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="D19" s="4"/>
+    <row r="19" spans="1:5" ht="60">
+      <c r="A19" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="D20" s="4"/>
+    <row r="20" spans="1:5" ht="60">
+      <c r="A20" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="D22" s="4"/>
+    <row r="21" spans="1:5" ht="120">
+      <c r="A21" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45">
+      <c r="A22" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
@@ -849,7 +2484,7 @@
       <c r="D45" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C45">
       <formula1>"Gestion, Analyse, Conception, Implémentation, "</formula1>
     </dataValidation>
@@ -860,25 +2495,82 @@
     <oddHeader>&amp;L&amp;"-,Gras"&amp;12Journal de travail&amp;C&amp;"-,Gras"&amp;14Runscape&amp;R&amp;"-,Gras"&amp;12TPI</oddHeader>
     <oddFooter>&amp;LPHILIBERT Alexandre&amp;CPage &amp;P&amp;R le &amp;D</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7">
+        <v>17.25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added zonning and wireframe for web client activity creation page (without GPX), Updated RapportDeTravail, Updated JournalDeBord
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI_PHILIBERT\Documentation\"/>
@@ -13,11 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -99,9 +98,6 @@
     <t>Je me suis aperçu que le format de retour de l'API n'est pas tout à fait adapté quand beaucoup d'enregistrement sont envoyés.</t>
   </si>
   <si>
-    <t>Étiquettes de lignes</t>
-  </si>
-  <si>
     <t>Total général</t>
   </si>
   <si>
@@ -129,13 +125,49 @@
     <t>Je crée le middleware de gestion des requêtes multipart. Cette fonctionnalitée est assez rapidement implémentée car j'avais déjà écrit d'autres middleware pour l'API précédament</t>
   </si>
   <si>
-    <t>Tests des modifications apportées sur le endpoint de création d'activités. J'effectue les tests avec des GPX fournit par Monsieur Glassey</t>
-  </si>
-  <si>
     <t>Modification de la création d'activité dans le modèle d'activité pour prendre en compte les champs traité par le middleware Formidable. J'ai créer une méthode dans la classe d'utility pour me permettre de changer le nom des propriétés d'un objet, cela va m'être utile lorsque les paramètres d'une requête HTTP ne correspondent pas aux noms de champs dans la base de données</t>
   </si>
   <si>
     <t>Je me suis rendu compte que les timestamps étaient décaler d'une heure, j'ai dabord cru que le problème vennait du format de timestmap que je fournissait en paramètre, mais le problème vennait en faite de la connection au serveur MySQL, je ne spécifait pas le timezone.</t>
+  </si>
+  <si>
+    <t>Tests des modifications apportées sur le endpoint de création d'activités. J'effectue les tests avec des GPX fournit par Monsieur Glassey. Après ces tests je lance la liste complète des tests pour vérifier que je n'ai pas casser une autre fonctionnalité de l'API</t>
+  </si>
+  <si>
+    <t>Analyse concurrentielle. J'ai eu quelques difficultés à trouver des sites d'analyse de GPX gratuits. J'ai trouvé beaucoup de sites qui permettent de dessiner des parcours sur une carte, mais ceux-ci ne m'interesse pas car mon projet ne consiste pas au dessin de parcours.</t>
+  </si>
+  <si>
+    <t>Ce matin j'ai trouvé un autre site d'analyse de GPX qui me semble plus complet que les 2 que j'avais trouvé hier, je l'ajoute à mon analyse concurentielle</t>
+  </si>
+  <si>
+    <t>Analyse des besoins pour la création d'un client web permettant la création d'activité sportives (sans GPX)</t>
+  </si>
+  <si>
+    <t>J'installe Pencil et Balsamiq qui me permettrons de réaliser les maquettes d'interfaces graphique. Je créé par la suite un zonning de la page de création d'activité (sans GPX). Je créer ensuite le wireframe de cette page.</t>
+  </si>
+  <si>
+    <t>Lorsque j'étais en train de créer  le wireframe, je me suis rendu compte que la page ne possèderait pas énormément d'élements contrairement aux sites que j'ai analyser dans mon analyse concurrentielle. Il me faudra donc faire attention à ne pas créer une interface trop vide</t>
+  </si>
+  <si>
+    <t>Entretien avec Monsieur Glassey pour préciser certains point du cahier des charges tel que la connexion au site web ainsi que les champs à saisir lors de la création d'activité</t>
+  </si>
+  <si>
+    <t>Je continue le wireframe de création d'activité sans GPX en prennant en considération les modifications discutées avec Monsieur Glassey</t>
+  </si>
+  <si>
+    <t>Je commente dans la documentation les types des champs que le sportif devra remplir pour créer son activité</t>
+  </si>
+  <si>
+    <t>Après quelques recherche sur internet je ne trouve pas de balise HTML input qui premettent de formater des timestamp, le seul champs que j'ai trouvé est le champs "datetime-local"mais le format n'est pas très convivial</t>
+  </si>
+  <si>
+    <t>Conception de la solution de rendu des pages web sur le client (Server side rendering, Client side rendering)</t>
+  </si>
+  <si>
+    <t>Je début cette conception avec une solution déjà éxistant, je trouve intéressant de voir quelle est la meilleure manière de la faire évoluer</t>
+  </si>
+  <si>
+    <t>Mise à jour du repository git, envoi du journal de bord et du rapport</t>
   </si>
 </sst>
 </file>
@@ -234,7 +266,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[PHILIBERT_JournalDeBord.xlsx]Feuil1!Tableau croisé dynamique2</c:name>
+    <c:name>[PHILIBERT_JournalDeBord.xlsx]Journal!Tableau croisé dynamique2</c:name>
     <c:fmtId val="3"/>
   </c:pivotSource>
   <c:chart>
@@ -520,6 +552,96 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -530,7 +652,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$3</c:f>
+              <c:f>Journal!$D$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -678,7 +800,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$4:$A$8</c:f>
+              <c:f>Journal!$C$52:$C$56</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -698,21 +820,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$4:$B$8</c:f>
+              <c:f>Journal!$D$52:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.25</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,14 +1513,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>676274</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:colOff>27352</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3438524</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>484553</xdr:colOff>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1424,16 +1546,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="PHILIBERT Alexandre" refreshedDate="43594.61665891204" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="44">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43595.611382986113" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="44">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-10T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-11T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="1.5"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1453,234 +1575,9 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="44">
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="1.5"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="1"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-07T00:00:00"/>
-    <n v="0.5"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <d v="2019-05-08T00:00:00"/>
-    <n v="0.75"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2019-05-08T00:00:00"/>
-    <n v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2019-05-08T00:00:00"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2019-05-08T00:00:00"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2019-05-09T00:00:00"/>
-    <n v="0.5"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2019-05-09T00:00:00"/>
-    <n v="0.5"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <d v="2019-05-09T00:00:00"/>
-    <n v="1"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <d v="2019-05-09T00:00:00"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2019-05-09T00:00:00"/>
-    <n v="1.5"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <d v="2019-05-09T00:00:00"/>
-    <n v="1"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="4"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="C51:D56" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1721,7 +1618,7 @@
   <dataFields count="1">
     <dataField name="Somme de Temps (h)" fld="1" baseField="0" baseItem="363412240"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="6">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -1736,6 +1633,54 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -2027,19 +1972,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2115,7 +2062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="30">
       <c r="A6" s="1">
         <v>43592</v>
       </c>
@@ -2129,7 +2076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45">
+    <row r="7" spans="1:8" ht="60">
       <c r="A7" s="1">
         <v>43592</v>
       </c>
@@ -2143,7 +2090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" s="1">
         <v>43592</v>
       </c>
@@ -2200,7 +2147,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="30">
       <c r="A12" s="1">
         <v>43592</v>
       </c>
@@ -2216,7 +2163,7 @@
       <c r="E12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="60">
+    <row r="13" spans="1:8" ht="105">
       <c r="A13" s="1">
         <v>43593</v>
       </c>
@@ -2231,7 +2178,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="60">
+    <row r="14" spans="1:8" ht="90">
       <c r="A14" s="1">
         <v>43593</v>
       </c>
@@ -2241,12 +2188,12 @@
       <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>27</v>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="60">
+    <row r="15" spans="1:8" ht="105">
       <c r="A15" s="1">
         <v>43593</v>
       </c>
@@ -2256,8 +2203,8 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -2271,7 +2218,7 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2288,14 +2235,14 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>29</v>
+      <c r="D17" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="1">
         <v>43594</v>
       </c>
@@ -2306,11 +2253,11 @@
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="90">
       <c r="A19" s="1">
         <v>43594</v>
       </c>
@@ -2321,11 +2268,11 @@
         <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="60">
+    <row r="20" spans="1:5" ht="90">
       <c r="A20" s="1">
         <v>43594</v>
       </c>
@@ -2336,11 +2283,11 @@
         <v>6</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="120">
+    <row r="21" spans="1:5" ht="165">
       <c r="A21" s="1">
         <v>43594</v>
       </c>
@@ -2351,13 +2298,13 @@
         <v>6</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="105">
       <c r="A22" s="1">
         <v>43594</v>
       </c>
@@ -2368,51 +2315,148 @@
         <v>6</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="D24" s="3"/>
+    <row r="23" spans="1:5" ht="120">
+      <c r="A23" s="1">
+        <v>43594</v>
+      </c>
+      <c r="B23">
+        <v>0.75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="75">
+      <c r="A24" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="D25" s="4"/>
+    <row r="25" spans="1:5" ht="45">
+      <c r="A25" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B25">
+        <v>0.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1"/>
-      <c r="D27" s="4"/>
+    <row r="26" spans="1:5" ht="135">
+      <c r="A26" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B26">
+        <v>1.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="75">
+      <c r="A27" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B27">
+        <v>0.25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1"/>
-      <c r="D28" s="4"/>
+    <row r="28" spans="1:5" ht="60">
+      <c r="A28" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1"/>
-      <c r="D31" s="4"/>
+    <row r="29" spans="1:5" ht="105">
+      <c r="A29" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60">
+      <c r="A30" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5">
@@ -2438,6 +2482,7 @@
     <row r="36" spans="1:5">
       <c r="A36" s="1"/>
       <c r="D36" s="4"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1"/>
@@ -2482,6 +2527,54 @@
     <row r="45" spans="1:5">
       <c r="A45" s="1"/>
       <c r="D45" s="4"/>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="C51" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="C52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="7">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="C54" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="7">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="C55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="7">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="7">
+        <v>23.75</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2490,87 +2583,14 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Gras"&amp;12Journal de travail&amp;C&amp;"-,Gras"&amp;14Runscape&amp;R&amp;"-,Gras"&amp;12TPI</oddHeader>
     <oddFooter>&amp;LPHILIBERT Alexandre&amp;CPage &amp;P&amp;R le &amp;D</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B8"/>
-  <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7">
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="7">
-        <v>17.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added first version of javascript framework, added activityCreation form, Updated RapportDeTravail and JournalDeBord
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>Mise à jour du repository git, envoi du journal de bord et du rapport</t>
+  </si>
+  <si>
+    <t>Conception de la solution permettant de servir des pages aux navigateurs et finalisation de la conception de la solution de rendu de pages retenue</t>
+  </si>
+  <si>
+    <t>Conception du framework de rendu de pages côté client. Je réfléchis à une solution permettant de gérer plusieurs pages d'une façon très simple mais efficace</t>
+  </si>
+  <si>
+    <t>Création du framework de génération des pages du côté navigateur. Je reprends les CSS que j'avais créer lors du pré-tpi pour ne pas perdre de temps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'implémente des fonctionnalités semblable à un site que j'avais créé à l'aide du framework VueJS car j'avais déjà rencontré les mêmes limitations </t>
+  </si>
+  <si>
+    <t>Création du formulaire de création d'activité</t>
   </si>
 </sst>
 </file>
@@ -652,7 +667,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$D$51</c:f>
+              <c:f>Journal!$D$80</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -800,7 +815,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$C$52:$C$56</c:f>
+              <c:f>Journal!$C$81:$C$85</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -820,7 +835,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$D$52:$D$56</c:f>
+              <c:f>Journal!$D$81:$D$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -828,13 +843,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,15 +1528,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27352</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>238663</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>101571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>484553</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>695864</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>92046</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1546,13 +1561,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43595.611382986113" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="44">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43599.452402430557" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="42">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-11T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-15T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1577,7 +1592,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="C51:D56" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="C80:D85" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1696,8 +1711,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E45">
-  <autoFilter ref="A1:E45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E43">
+  <autoFilter ref="A1:E43"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -1972,18 +1987,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
@@ -2062,7 +2077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>43592</v>
       </c>
@@ -2076,7 +2091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60">
+    <row r="7" spans="1:8" ht="45">
       <c r="A7" s="1">
         <v>43592</v>
       </c>
@@ -2090,7 +2105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8" ht="20.25" customHeight="1">
       <c r="A8" s="1">
         <v>43592</v>
       </c>
@@ -2163,7 +2178,7 @@
       <c r="E12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="105">
+    <row r="13" spans="1:8" ht="82.5" customHeight="1">
       <c r="A13" s="1">
         <v>43593</v>
       </c>
@@ -2178,7 +2193,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="90">
+    <row r="14" spans="1:8" ht="79.5" customHeight="1">
       <c r="A14" s="1">
         <v>43593</v>
       </c>
@@ -2193,7 +2208,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="105">
+    <row r="15" spans="1:8" ht="82.5" customHeight="1">
       <c r="A15" s="1">
         <v>43593</v>
       </c>
@@ -2208,7 +2223,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="60">
+    <row r="16" spans="1:8" ht="63" customHeight="1">
       <c r="A16" s="1">
         <v>43593</v>
       </c>
@@ -2242,7 +2257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="30">
       <c r="A18" s="1">
         <v>43594</v>
       </c>
@@ -2257,7 +2272,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="90">
+    <row r="19" spans="1:5" ht="75" customHeight="1">
       <c r="A19" s="1">
         <v>43594</v>
       </c>
@@ -2272,7 +2287,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="90">
+    <row r="20" spans="1:5" ht="65.25" customHeight="1">
       <c r="A20" s="1">
         <v>43594</v>
       </c>
@@ -2287,7 +2302,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="165">
+    <row r="21" spans="1:5" ht="126.75" customHeight="1">
       <c r="A21" s="1">
         <v>43594</v>
       </c>
@@ -2304,7 +2319,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="105">
+    <row r="22" spans="1:5" ht="83.25" customHeight="1">
       <c r="A22" s="1">
         <v>43594</v>
       </c>
@@ -2319,7 +2334,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="120">
+    <row r="23" spans="1:5" ht="94.5" customHeight="1">
       <c r="A23" s="1">
         <v>43594</v>
       </c>
@@ -2333,7 +2348,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="75">
+    <row r="24" spans="1:5" ht="52.5" customHeight="1">
       <c r="A24" s="1">
         <v>43595</v>
       </c>
@@ -2348,7 +2363,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="45">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="1">
         <v>43595</v>
       </c>
@@ -2363,7 +2378,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="135">
+    <row r="26" spans="1:5" ht="126" customHeight="1">
       <c r="A26" s="1">
         <v>43595</v>
       </c>
@@ -2380,7 +2395,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="75">
+    <row r="27" spans="1:5" ht="59.25" customHeight="1">
       <c r="A27" s="1">
         <v>43595</v>
       </c>
@@ -2395,7 +2410,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="60">
+    <row r="28" spans="1:5" ht="49.5" customHeight="1">
       <c r="A28" s="1">
         <v>43595</v>
       </c>
@@ -2410,7 +2425,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="105">
+    <row r="29" spans="1:5" ht="92.25" customHeight="1">
       <c r="A29" s="1">
         <v>43595</v>
       </c>
@@ -2459,24 +2474,66 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1"/>
-      <c r="D32" s="4"/>
+    <row r="32" spans="1:5" ht="45">
+      <c r="A32" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1"/>
-      <c r="D33" s="4"/>
+    <row r="33" spans="1:5" ht="45">
+      <c r="A33" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1"/>
-      <c r="D35" s="4"/>
+    <row r="34" spans="1:5" ht="135">
+      <c r="A34" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B34">
+        <v>1.5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45">
+      <c r="A35" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5">
@@ -2519,66 +2576,57 @@
       <c r="D43" s="4"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="51" spans="3:4">
-      <c r="C51" s="5" t="s">
+    <row r="80" spans="3:4">
+      <c r="C80" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D80" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="3:4">
-      <c r="C52" s="6" t="s">
+    <row r="81" spans="3:4">
+      <c r="C81" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D81" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="3:4">
-      <c r="C53" s="6" t="s">
+    <row r="82" spans="3:4">
+      <c r="C82" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="7">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4">
-      <c r="C54" s="6" t="s">
+      <c r="D82" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4">
+      <c r="C83" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D83" s="7">
         <v>6.75</v>
       </c>
     </row>
-    <row r="55" spans="3:4">
-      <c r="C55" s="6" t="s">
+    <row r="84" spans="3:4">
+      <c r="C84" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="7">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4">
-      <c r="C56" s="6" t="s">
+      <c r="D84" s="7">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4">
+      <c r="C85" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="7">
-        <v>23.75</v>
+      <c r="D85" s="7">
+        <v>27.25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C43">
       <formula1>"Gestion, Analyse, Conception, Implémentation, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added async XHR request for activity location and type on activity creation form
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>Création du formulaire de création d'activité</t>
+  </si>
+  <si>
+    <t>Continuation de la création du formulaire de création d'activité, Ajout des requêtes XHR sur les différentes ressources (pays, lieu) ainsi que création de la requête d'envoi de l'activité.Création d'une méthode d'utility pour l'envoi de requêtes XHR</t>
+  </si>
+  <si>
+    <t>J'ai créé une méthode que je pourrais réutiliser pour toutes les requêtes XHR que j'effectuerais depuis le client</t>
+  </si>
+  <si>
+    <t>Mise à jour du repository, mise à jour du journal de bord</t>
   </si>
 </sst>
 </file>
@@ -846,10 +855,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.75</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1561,7 +1570,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43599.452402430557" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="42">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43599.699974074072" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="42">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
@@ -1989,14 +1998,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
@@ -2021,7 +2030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" s="1">
         <v>43592</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="1">
         <v>43592</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="75">
       <c r="A5" s="1">
         <v>43592</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" s="1">
         <v>43592</v>
       </c>
@@ -2091,7 +2100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45">
+    <row r="7" spans="1:8" ht="135">
       <c r="A7" s="1">
         <v>43592</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8" ht="60">
       <c r="A10" s="1">
         <v>43592</v>
       </c>
@@ -2162,7 +2171,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="60">
       <c r="A12" s="1">
         <v>43592</v>
       </c>
@@ -2257,7 +2266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="75">
       <c r="A18" s="1">
         <v>43594</v>
       </c>
@@ -2363,7 +2372,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="90">
       <c r="A25" s="1">
         <v>43595</v>
       </c>
@@ -2442,7 +2451,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60">
+    <row r="30" spans="1:5" ht="90">
       <c r="A30" s="1">
         <v>43595</v>
       </c>
@@ -2459,7 +2468,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="60">
       <c r="A31" s="1">
         <v>43595</v>
       </c>
@@ -2474,7 +2483,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="45">
+    <row r="32" spans="1:5" ht="120">
       <c r="A32" s="1">
         <v>43599</v>
       </c>
@@ -2489,7 +2498,7 @@
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="45">
+    <row r="33" spans="1:5" ht="135">
       <c r="A33" s="1">
         <v>43599</v>
       </c>
@@ -2536,19 +2545,51 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1"/>
-      <c r="D36" s="4"/>
+    <row r="36" spans="1:5" ht="45">
+      <c r="A36" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1"/>
-      <c r="D38" s="4"/>
+    <row r="37" spans="1:5" ht="225">
+      <c r="A37" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B37">
+        <v>1.5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="60">
+      <c r="A38" s="1">
+        <v>43599</v>
+      </c>
+      <c r="B38">
+        <v>0.25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5">
@@ -2605,7 +2646,7 @@
         <v>4</v>
       </c>
       <c r="D83" s="7">
-        <v>6.75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="3:4">
@@ -2613,7 +2654,7 @@
         <v>6</v>
       </c>
       <c r="D84" s="7">
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="85" spans="3:4">
@@ -2621,7 +2662,7 @@
         <v>23</v>
       </c>
       <c r="D85" s="7">
-        <v>27.25</v>
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Users are now able to create Activties (without GPX) from the web interface Updated RapportDeTravail to reflect part taken from PRE-TPI Updated JournalDeBord with tasks done today Added example.vsdx with an example of MLD nomenclature
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,27 @@
   </si>
   <si>
     <t>Mise à jour du repository, mise à jour du journal de bord</t>
+  </si>
+  <si>
+    <t>J'apporte les modifications disuctées hier avec Monsieur Glassey au rapport de travail (MCD, MLD, objectifs)</t>
+  </si>
+  <si>
+    <t>J'ai du modifier la forme du rapport de travail pour indiquer que certains éléments (MCD, MLD) étaient repris du pré-tpi</t>
+  </si>
+  <si>
+    <t>Ajout d'une issue pour la route "notfound" sur le client web</t>
+  </si>
+  <si>
+    <t>Finalisation du formulaire de création des activités sur l'interface graphique. Il est désormais possible de créer des requêtes sur le client web</t>
+  </si>
+  <si>
+    <t>Je réfléchis à la façon dont je vais retourner les erreurs aux sportifs si une erreur survient du côté de l'API</t>
+  </si>
+  <si>
+    <t>Tests de la création d'activités, je notes les améliorations possibles ainsi que les erreurs restantes</t>
+  </si>
+  <si>
+    <t>Il est possbile, sur firefox, d'envoyer une requête contenant des dates de début et de fin d'activité érronés. La requête est néanmoins stoppée sur le serveur lors de la validation du format de timestamp</t>
   </si>
 </sst>
 </file>
@@ -237,10 +258,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -252,6 +269,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +699,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$D$80</c:f>
+              <c:f>Journal!$D$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -824,7 +847,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$C$81:$C$85</c:f>
+              <c:f>Journal!$C$51:$C$55</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -844,7 +867,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$D$81:$D$85</c:f>
+              <c:f>Journal!$D$51:$D$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -852,13 +875,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.5</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1537,15 +1560,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238663</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>101571</xdr:rowOff>
+      <xdr:colOff>664487</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>168807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>695864</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>92046</xdr:rowOff>
+      <xdr:colOff>1121688</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>159282</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1570,13 +1593,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43599.699974074072" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="42">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43600.497616666667" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="42">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-15T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-16T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1600,8 +1623,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="C80:D85" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="C50:D55" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1996,18 +2019,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
@@ -2030,639 +2053,664 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
-      <c r="A2" s="1">
+    <row r="2" spans="1:8" s="1" customFormat="1">
+      <c r="A2" s="6">
         <v>43592</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A3" s="1">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A3" s="6">
         <v>43592</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0.5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="1">
+    <row r="4" spans="1:8" s="1" customFormat="1">
+      <c r="A4" s="6">
         <v>43592</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1.5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75">
-      <c r="A5" s="1">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A5" s="6">
         <v>43592</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="1">
+    <row r="6" spans="1:8" s="1" customFormat="1">
+      <c r="A6" s="6">
         <v>43592</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="135">
-      <c r="A7" s="1">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="45">
+      <c r="A7" s="6">
         <v>43592</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A8" s="1">
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A8" s="6">
         <v>43592</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0.5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A9" s="1">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="6">
         <v>43592</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>0.5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60">
-      <c r="A10" s="1">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A10" s="6">
         <v>43592</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="44.25" customHeight="1">
-      <c r="A11" s="1">
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="44.25" customHeight="1">
+      <c r="A11" s="6">
         <v>43592</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="60">
-      <c r="A12" s="1">
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A12" s="6">
         <v>43592</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="82.5" customHeight="1">
-      <c r="A13" s="1">
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A13" s="6">
         <v>43593</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.75</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="79.5" customHeight="1">
-      <c r="A14" s="1">
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="79.5" customHeight="1">
+      <c r="A14" s="6">
         <v>43593</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="82.5" customHeight="1">
-      <c r="A15" s="1">
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A15" s="6">
         <v>43593</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="63" customHeight="1">
-      <c r="A16" s="1">
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="63" customHeight="1">
+      <c r="A16" s="6">
         <v>43593</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="105">
-      <c r="A17" s="1">
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="105">
+      <c r="A17" s="6">
         <v>43594</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.5</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="75">
-      <c r="A18" s="1">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A18" s="6">
         <v>43594</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="75" customHeight="1">
-      <c r="A19" s="1">
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="75" customHeight="1">
+      <c r="A19" s="6">
         <v>43594</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="65.25" customHeight="1">
-      <c r="A20" s="1">
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="65.25" customHeight="1">
+      <c r="A20" s="6">
         <v>43594</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="126.75" customHeight="1">
-      <c r="A21" s="1">
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="126.75" customHeight="1">
+      <c r="A21" s="6">
         <v>43594</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="83.25" customHeight="1">
-      <c r="A22" s="1">
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="83.25" customHeight="1">
+      <c r="A22" s="6">
         <v>43594</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="94.5" customHeight="1">
-      <c r="A23" s="1">
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A23" s="6">
         <v>43594</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.75</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="52.5" customHeight="1">
-      <c r="A24" s="1">
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1">
+      <c r="A24" s="6">
         <v>43595</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.5</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="90">
-      <c r="A25" s="1">
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A25" s="6">
         <v>43595</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>0.5</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="126" customHeight="1">
-      <c r="A26" s="1">
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" ht="126" customHeight="1">
+      <c r="A26" s="6">
         <v>43595</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>1.5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="59.25" customHeight="1">
-      <c r="A27" s="1">
+    <row r="27" spans="1:5" s="1" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A27" s="6">
         <v>43595</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>0.25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" ht="49.5" customHeight="1">
-      <c r="A28" s="1">
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1">
+      <c r="A28" s="6">
         <v>43595</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0.5</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="92.25" customHeight="1">
-      <c r="A29" s="1">
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1" ht="92.25" customHeight="1">
+      <c r="A29" s="6">
         <v>43595</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>0.5</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="90">
-      <c r="A30" s="1">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A30" s="6">
         <v>43595</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60">
-      <c r="A31" s="1">
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A31" s="6">
         <v>43595</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>0.5</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" ht="120">
-      <c r="A32" s="1">
+    </row>
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A32" s="6">
         <v>43599</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>0.5</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5" ht="135">
-      <c r="A33" s="1">
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A33" s="6">
         <v>43599</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5" ht="135">
-      <c r="A34" s="1">
+    </row>
+    <row r="34" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A34" s="6">
         <v>43599</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>1.5</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="45">
-      <c r="A35" s="1">
+    <row r="35" spans="1:5" s="1" customFormat="1">
+      <c r="A35" s="6">
         <v>43599</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5" ht="45">
-      <c r="A36" s="1">
+    </row>
+    <row r="36" spans="1:5" s="1" customFormat="1">
+      <c r="A36" s="6">
         <v>43599</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:5" ht="225">
-      <c r="A37" s="1">
+    </row>
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="75">
+      <c r="A37" s="6">
         <v>43599</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>1.5</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="60">
-      <c r="A38" s="1">
+    <row r="38" spans="1:5" s="1" customFormat="1">
+      <c r="A38" s="6">
         <v>43599</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>0.25</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="80" spans="3:4">
-      <c r="C80" s="5" t="s">
+    </row>
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A39" s="6">
+        <v>43600</v>
+      </c>
+      <c r="B39" s="1">
         <v>1</v>
       </c>
-      <c r="D80" t="s">
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A40" s="6">
+        <v>43600</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A41" s="6">
+        <v>43600</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="75">
+      <c r="A42" s="6">
+        <v>43600</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="1" customFormat="1">
+      <c r="A43" s="6"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="3:4">
-      <c r="C81" s="6" t="s">
+    <row r="51" spans="3:4">
+      <c r="C51" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D51" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="3:4">
-      <c r="C82" s="6" t="s">
+    <row r="52" spans="3:4">
+      <c r="C52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4">
-      <c r="C83" s="6" t="s">
+      <c r="D52" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D53" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="3:4">
-      <c r="C84" s="6" t="s">
+    <row r="54" spans="3:4">
+      <c r="C54" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="7">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="85" spans="3:4">
-      <c r="C85" s="6" t="s">
+      <c r="D54" s="5">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="C55" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D85" s="7">
-        <v>30.5</v>
+      <c r="D55" s="5">
+        <v>34.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added activity creation with GPX in form, Added activity dashboard with ressource mapping for places, activityType, Created new endpoint for places retreival
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,33 @@
   </si>
   <si>
     <t>Il est possbile, sur firefox, d'envoyer une requête contenant des dates de début et de fin d'activité érronés. La requête est néanmoins stoppée sur le serveur lors de la validation du format de timestamp</t>
+  </si>
+  <si>
+    <t>Gestion des erreurs sur le client</t>
+  </si>
+  <si>
+    <t>Correction d'un bug ou l'un des appels XHR ne s'effectuait pas aux chargement de la page (lieux)</t>
+  </si>
+  <si>
+    <t>Conception de la création d'une activité sportive à l'aide de l'interface et d'un GPX</t>
+  </si>
+  <si>
+    <t>Ajout du champ gpx au formulaire de création d'activité. Je dois légérement changer la logique de création de requête, mais cette tâche est assez rapidement réalisé car le back-end est déjà fonctionnel</t>
+  </si>
+  <si>
+    <t>Analyse des besoins d'une page regroupant toutes les activités réalisés par un sportif</t>
+  </si>
+  <si>
+    <t>Création du wireframe de la page de dashboard</t>
+  </si>
+  <si>
+    <t>Conception de la récupération des différentes ressources nécessaires pour l'affichage des activités tel que le lieu et le type d'activité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beauoup de solutions existent pour faire le mapping des ressources. J'ai décidé dans un premier temps d'implémenter une solution simple et pas forcément très optimisée. Je pourrais par la suite revenir sur cette problèmatique et y apporté une solution plus optimisée </t>
+  </si>
+  <si>
+    <t>Création de la page de dashboard. Les problèmes que je pensais rencontrer lors de la conception se sont manifestés. J'ai implémenter la solution envisagé. Des améliorations restent néanmoins possible</t>
   </si>
 </sst>
 </file>
@@ -699,7 +726,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$D$50</c:f>
+              <c:f>Journal!$D$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -847,7 +874,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$C$51:$C$55</c:f>
+              <c:f>Journal!$C$60:$C$64</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -867,21 +894,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$D$51:$D$55</c:f>
+              <c:f>Journal!$D$60:$D$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.25</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1561,13 +1588,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>664487</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>168807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1121688</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>159282</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1593,13 +1620,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43600.497616666667" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="42">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43601.703439120371" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="52">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-16T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-17T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1623,8 +1650,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="C50:D55" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="C59:D64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1743,8 +1770,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E43">
-  <autoFilter ref="A1:E43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E53">
+  <autoFilter ref="A1:E53"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -2019,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2032,6 +2059,8 @@
     <col min="4" max="4" width="51.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
@@ -2661,61 +2690,184 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1">
-      <c r="A43" s="6"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="50" spans="3:4">
-      <c r="C50" s="3" t="s">
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A43" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="1" customFormat="1">
+      <c r="A44" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A45" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B45" s="1">
         <v>1</v>
       </c>
-      <c r="D50" t="s">
+      <c r="C45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A46" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A47" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="1" customFormat="1">
+      <c r="A48" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="1" customFormat="1" ht="105">
+      <c r="A49" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A50" s="6">
+        <v>43601</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="1" customFormat="1">
+      <c r="A51" s="6"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" s="1" customFormat="1">
+      <c r="A52" s="6"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1">
+      <c r="A53" s="6"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="C59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:4">
-      <c r="C51" s="4" t="s">
+    <row r="60" spans="1:5">
+      <c r="C60" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4">
-      <c r="C52" s="4" t="s">
+      <c r="D60" s="5">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="C61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D61" s="5">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="C62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="3:4">
-      <c r="C53" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4">
-      <c r="C54" s="4" t="s">
+    <row r="63" spans="1:5">
+      <c r="C63" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="5">
-        <v>13.25</v>
-      </c>
-    </row>
-    <row r="55" spans="3:4">
-      <c r="C55" s="4" t="s">
+      <c r="D63" s="5">
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="C64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D55" s="5">
-        <v>34.25</v>
+      <c r="D64" s="5">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C43 C44">
       <formula1>"Gestion, Analyse, Conception, Implémentation, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added new wireframe for activity viewing, Updated JournalDeBord, Updated RapportDeTravail with Map service analysis, Fixed router issue for notfound path, Added menu highlight for current page
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -240,6 +240,33 @@
   </si>
   <si>
     <t>Création de la page de dashboard. Les problèmes que je pensais rencontrer lors de la conception se sont manifestés. J'ai implémenter la solution envisagé. Des améliorations restent néanmoins possible</t>
+  </si>
+  <si>
+    <t>Corrections de bug dans le router du client web, à certains moment les pages n'étaient pas changées</t>
+  </si>
+  <si>
+    <t>Ajout du highlight de l'élément courant dans le menu de l'application</t>
+  </si>
+  <si>
+    <t>J'ai dû modifier le header pour y ajouter une méthode permettant de notifier les items du menu lorsqu'un changement de page a lieu</t>
+  </si>
+  <si>
+    <t>J'ai trouvé un site web qui mets en avant 3 possibilités pour améliorer les relations entre les ressources de l'API</t>
+  </si>
+  <si>
+    <t>Conception d'améliorations possibles pour les requêtes de selection d'activités. Je documente les différentes options qui sont disponible pour améliorer les relations entre les ressources</t>
+  </si>
+  <si>
+    <t>Analyse des besoins du sportif pour la fonctionnalité de visualisation d'activités sous forme de carte</t>
+  </si>
+  <si>
+    <t>Choix du fournisseur de carte (Google Maps, OSM) et explications de ce choix</t>
+  </si>
+  <si>
+    <t>Je réfléchis à une solution pour garder l'identifiant d'une activité lors du changement de page. Cela permettra également au sportif d'enregistrer la page du parcours d'une activité dans ses favoris par exemple</t>
+  </si>
+  <si>
+    <t>Pseudo code pour le dessin du parcours sur la carte Google Maps. Je m'inspire du tutoriel trouvé sur la documentation de l'API Polylines de Maps</t>
   </si>
 </sst>
 </file>
@@ -726,7 +753,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$D$59</c:f>
+              <c:f>Journal!$D$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -874,7 +901,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$C$60:$C$64</c:f>
+              <c:f>Journal!$C$65:$C$69</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -894,21 +921,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$D$60:$D$64</c:f>
+              <c:f>Journal!$D$65:$D$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.25</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.25</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,13 +1615,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>664487</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>168807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1121688</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>159282</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1620,13 +1647,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43601.703439120371" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="52">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43602.614842708332" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="57">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-17T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-18T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1650,8 +1677,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="C59:D64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="C64:D69" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1770,8 +1797,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E53">
-  <autoFilter ref="A1:E53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E58">
+  <autoFilter ref="A1:E58"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -2046,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:D64"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2059,9 +2086,9 @@
     <col min="4" max="4" width="51.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2805,64 +2832,160 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="1" customFormat="1">
-      <c r="A51" s="6"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" s="1" customFormat="1">
-      <c r="A52" s="6"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" s="1" customFormat="1">
-      <c r="A53" s="6"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="C59" s="3" t="s">
+    <row r="51" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A51" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B51" s="1">
         <v>1</v>
       </c>
-      <c r="D59" t="s">
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A52" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A53" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A54" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A55" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A56" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A57" s="6">
+        <v>43602</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1">
+      <c r="A58" s="6"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="C64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
-      <c r="C60" s="4" t="s">
+    <row r="65" spans="3:4">
+      <c r="C65" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="5">
-        <v>5.25</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="C61" s="4" t="s">
+      <c r="D65" s="5">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4">
+      <c r="C66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="5">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="C62" s="4" t="s">
+      <c r="D66" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4">
+      <c r="C67" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D67" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
-      <c r="C63" s="4" t="s">
+    <row r="68" spans="3:4">
+      <c r="C68" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="5">
-        <v>17.25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="C64" s="4" t="s">
+      <c r="D68" s="5">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4">
+      <c r="C69" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="5">
-        <v>41</v>
+      <c r="D69" s="5">
+        <v>46.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in website router where no page would load if not defined in url, Modified Wireframes, Created postman config doc
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="27" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -267,6 +267,30 @@
   </si>
   <si>
     <t>Pseudo code pour le dessin du parcours sur la carte Google Maps. Je m'inspire du tutoriel trouvé sur la documentation de l'API Polylines de Maps</t>
+  </si>
+  <si>
+    <t>Déploiement de l'application sur AWS</t>
+  </si>
+  <si>
+    <t>Je ne pensais pas prendre autant de temps à deployer l'application. J'ai rencontré quelques bugs lors des tests que j'ai pu corriger.</t>
+  </si>
+  <si>
+    <t>Lecture du protocole de visite du deuxième expert</t>
+  </si>
+  <si>
+    <t>Création de la page de visualisation de l'activité sous forme de carte, ajout de Google maps dans la page sous forme de Proof of concept dans un premier temps</t>
+  </si>
+  <si>
+    <t>Je déplace la plannification initiale en annexe</t>
+  </si>
+  <si>
+    <t>Meeting hebdomadaire avec Monsieur Glassey. Visite du second expert</t>
+  </si>
+  <si>
+    <t>Écriture d'une documentation de configuration de postman suite à la demande du chef de projet et du second expert</t>
+  </si>
+  <si>
+    <t>Correction d'un bug dans le routeur sur le client web lorsque aucune page n'était définie dans l'url</t>
   </si>
 </sst>
 </file>
@@ -753,7 +777,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$D$64</c:f>
+              <c:f>Journal!$G$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -901,7 +925,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$C$65:$C$69</c:f>
+              <c:f>Journal!$F$83:$F$87</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -921,21 +945,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$D$65:$D$69</c:f>
+              <c:f>Journal!$G$83:$G$87</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.5</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.75</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1614,15 +1638,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>664487</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>168807</xdr:rowOff>
+      <xdr:colOff>721637</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>111657</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1121688</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>159282</xdr:rowOff>
+      <xdr:colOff>1235988</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>102132</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1647,13 +1671,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43602.614842708332" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="57">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43606.703912731478" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-18T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-22T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1677,8 +1701,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="C64:D69" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="F82:G87" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1797,8 +1821,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E58">
-  <autoFilter ref="A1:E58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E65">
+  <autoFilter ref="A1:E65"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -2073,10 +2097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2085,7 +2109,8 @@
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="51.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -2936,56 +2961,157 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="1" customFormat="1">
-      <c r="A58" s="6"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="C64" s="3" t="s">
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A58" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="1" customFormat="1">
+      <c r="A59" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="1" customFormat="1">
+      <c r="A60" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A61" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B61" s="1">
         <v>1</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A62" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A63" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A64" s="6">
+        <v>43606</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="1" customFormat="1">
+      <c r="A65" s="6"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="82" spans="6:7">
+      <c r="F82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G82" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
-      <c r="C65" s="4" t="s">
+    <row r="83" spans="6:7">
+      <c r="F83" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="5">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4">
-      <c r="C66" s="4" t="s">
+      <c r="G83" s="5">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="84" spans="6:7">
+      <c r="F84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="5">
+      <c r="G84" s="5">
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
-      <c r="C67" s="4" t="s">
+    <row r="85" spans="6:7">
+      <c r="F85" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4">
-      <c r="C68" s="4" t="s">
+      <c r="G85" s="5">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="86" spans="6:7">
+      <c r="F86" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="5">
-        <v>18.75</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4">
-      <c r="C69" s="4" t="s">
+      <c r="G86" s="5">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="87" spans="6:7">
+      <c r="F87" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D69" s="5">
-        <v>46.25</v>
+      <c r="G87" s="5">
+        <v>52.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sequence diagram for activity Page
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -14,9 +14,12 @@
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$72</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="27" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -291,6 +294,18 @@
   </si>
   <si>
     <t>Correction d'un bug dans le routeur sur le client web lorsque aucune page n'était définie dans l'url</t>
+  </si>
+  <si>
+    <t>Écriture du use case et des scenarii d'affichage de la page d'interprétation du parcours</t>
+  </si>
+  <si>
+    <t>Je me demande comment décrire dans les scenarii que certaines actions sont réalisées de manières asynchrones. Je pense créer un diagramme de séquence</t>
+  </si>
+  <si>
+    <t>Création de la page d'affichage d'une activité en y intégrant le POC de la carte</t>
+  </si>
+  <si>
+    <t>Création d'un diagramme de séquence décrivant le processus d'affichage d'une activité</t>
   </si>
 </sst>
 </file>
@@ -777,7 +792,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$G$82</c:f>
+              <c:f>Journal!$G$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -925,7 +940,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$F$83:$F$87</c:f>
+              <c:f>Journal!$F$91:$F$95</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -945,7 +960,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$G$83:$G$87</c:f>
+              <c:f>Journal!$G$91:$G$95</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -953,13 +968,13 @@
                   <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1638,15 +1653,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>721637</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>111657</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>178332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1235988</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>102132</xdr:rowOff>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>168807</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1671,13 +1686,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43606.703912731478" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43607.388725231482" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="72">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-22T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-23T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1701,8 +1716,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="F82:G87" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="F90:G95" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1821,8 +1836,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E65">
-  <autoFilter ref="A1:E65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E73">
+  <autoFilter ref="A1:E73"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -2097,17 +2112,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A73" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45" customWidth="1"/>
     <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
@@ -3062,60 +3077,122 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="1" customFormat="1">
-      <c r="A65" s="6"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="82" spans="6:7">
-      <c r="F82" s="3" t="s">
+    <row r="65" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A65" s="6">
+        <v>43607</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A66" s="6">
+        <v>43607</v>
+      </c>
+      <c r="B66" s="1">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
+      <c r="C66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A67" s="6">
+        <v>43607</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1">
+      <c r="A68" s="6"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:5" s="1" customFormat="1">
+      <c r="A69" s="6"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:5" s="1" customFormat="1">
+      <c r="A70" s="6"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:5" s="1" customFormat="1">
+      <c r="A71" s="6"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:5" s="1" customFormat="1">
+      <c r="A72" s="6"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" s="1" customFormat="1">
+      <c r="A73" s="6"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="90" spans="6:7">
+      <c r="F90" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G90" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="6:7">
-      <c r="F83" s="4" t="s">
+    <row r="91" spans="6:7">
+      <c r="F91" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G83" s="5">
+      <c r="G91" s="5">
         <v>5.75</v>
       </c>
     </row>
-    <row r="84" spans="6:7">
-      <c r="F84" s="4" t="s">
+    <row r="92" spans="6:7">
+      <c r="F92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G84" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="85" spans="6:7">
-      <c r="F85" s="4" t="s">
+      <c r="G92" s="5">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="93" spans="6:7">
+      <c r="F93" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G85" s="5">
+      <c r="G93" s="5">
         <v>10.25</v>
       </c>
     </row>
-    <row r="86" spans="6:7">
-      <c r="F86" s="4" t="s">
+    <row r="94" spans="6:7">
+      <c r="F94" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G86" s="5">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="87" spans="6:7">
-      <c r="F87" s="4" t="s">
+      <c r="G94" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="6:7">
+      <c r="F95" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G87" s="5">
-        <v>52.5</v>
+      <c r="G95" s="5">
+        <v>53.5</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C43 C44">
       <formula1>"Gestion, Analyse, Conception, Implémentation, "</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Added way to pass parameter to pages constructor functions, Added POC for pace calculation
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -15,11 +15,11 @@
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$73</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>Création d'un diagramme de séquence décrivant le processus d'affichage d'une activité</t>
+  </si>
+  <si>
+    <t>Modification du router du client web pour pouvoir passer des parmètres aux pages à charger</t>
+  </si>
+  <si>
+    <t>Rendu du document de configuration de Postman sur Trello</t>
   </si>
 </sst>
 </file>
@@ -792,7 +798,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$G$90</c:f>
+              <c:f>Journal!$G$91</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -940,7 +946,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$F$91:$F$95</c:f>
+              <c:f>Journal!$F$92:$F$96</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -960,7 +966,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$G$91:$G$95</c:f>
+              <c:f>Journal!$G$92:$G$96</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -971,10 +977,10 @@
                   <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.25</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,13 +1660,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>178332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>168807</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1686,7 +1692,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43607.388725231482" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="72">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43607.504068518516" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="73">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
@@ -1716,8 +1722,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="F90:G95" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
+  <location ref="F91:G96" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1836,8 +1842,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E73">
-  <autoFilter ref="A1:E73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E74">
+  <autoFilter ref="A1:E74"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
     <tableColumn id="2" name="Temps (h)"/>
@@ -2112,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A73" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScale="70" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2219,7 +2225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="45">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="60">
       <c r="A7" s="6">
         <v>43592</v>
       </c>
@@ -2481,7 +2487,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A25" s="6">
         <v>43595</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A32" s="6">
         <v>43599</v>
       </c>
@@ -2602,7 +2608,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A33" s="6">
         <v>43599</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" ht="75">
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="90">
       <c r="A37" s="6">
         <v>43599</v>
       </c>
@@ -2678,7 +2684,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="1" customFormat="1">
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A38" s="6">
         <v>43599</v>
       </c>
@@ -2723,7 +2729,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A41" s="6">
         <v>43600</v>
       </c>
@@ -2757,7 +2763,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A43" s="6">
         <v>43601</v>
       </c>
@@ -2799,7 +2805,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="46" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A46" s="6">
         <v>43601</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="50" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A50" s="6">
         <v>43601</v>
       </c>
@@ -2872,7 +2878,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="51" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A51" s="6">
         <v>43602</v>
       </c>
@@ -2920,7 +2926,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A54" s="6">
         <v>43602</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A56" s="6">
         <v>43602</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A57" s="6">
         <v>43602</v>
       </c>
@@ -3007,7 +3013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="1" customFormat="1">
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A60" s="6">
         <v>43606</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="61" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A61" s="6">
         <v>43606</v>
       </c>
@@ -3063,7 +3069,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="64" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A64" s="6">
         <v>43606</v>
       </c>
@@ -3112,20 +3118,43 @@
       <c r="A67" s="6">
         <v>43607</v>
       </c>
+      <c r="B67" s="1">
+        <v>0.5</v>
+      </c>
       <c r="C67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A68" s="6">
+        <v>43607</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A69" s="6">
+        <v>43607</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" s="1" customFormat="1">
-      <c r="A68" s="6"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" s="1" customFormat="1">
-      <c r="A69" s="6"/>
-      <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:5" s="1" customFormat="1">
       <c r="A70" s="6"/>
@@ -3143,52 +3172,56 @@
       <c r="A73" s="6"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="90" spans="6:7">
-      <c r="F90" s="3" t="s">
+    <row r="74" spans="1:5" s="1" customFormat="1">
+      <c r="A74" s="6"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="91" spans="6:7">
+      <c r="F91" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="91" spans="6:7">
-      <c r="F91" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G91" s="5">
-        <v>5.75</v>
       </c>
     </row>
     <row r="92" spans="6:7">
       <c r="F92" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G92" s="5">
-        <v>15.5</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="93" spans="6:7">
       <c r="F93" s="4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G93" s="5">
-        <v>10.25</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="94" spans="6:7">
       <c r="F94" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G94" s="5">
-        <v>22</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="95" spans="6:7">
       <c r="F95" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="5">
+        <v>23.75</v>
+      </c>
+    </row>
+    <row r="96" spans="6:7">
+      <c r="F96" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G95" s="5">
-        <v>53.5</v>
+      <c r="G96" s="5">
+        <v>55.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pace stats on activity page, Fixed a bug in SQL query where activity position where not returned in the correct order
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -15,11 +15,11 @@
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$73</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$69</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId2"/>
+    <pivotCache cacheId="3" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -308,10 +308,19 @@
     <t>Création d'un diagramme de séquence décrivant le processus d'affichage d'une activité</t>
   </si>
   <si>
-    <t>Modification du router du client web pour pouvoir passer des parmètres aux pages à charger</t>
-  </si>
-  <si>
     <t>Rendu du document de configuration de Postman sur Trello</t>
+  </si>
+  <si>
+    <t>Modification du routeur du client web pour pouvoir passer des parmètres aux pages à charger</t>
+  </si>
+  <si>
+    <t>Je continue la cration de la page d'affichage d'une activité, j'ai écris une fonction utilisant le module node gps-distance pour calculer le pace par km du côté client</t>
+  </si>
+  <si>
+    <t>Documentation de la fonction calculant le pace, j'avais des doutes sur le temps d'exécution de la fonction sachant que lors du calcul de certains parcours plus de 20'000 points devaient être calculés.</t>
+  </si>
+  <si>
+    <t>Création d'un test sur le endpoint des positions d'une activité</t>
   </si>
 </sst>
 </file>
@@ -378,12 +387,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -798,7 +827,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$G$91</c:f>
+              <c:f>Journal!$H$84</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -946,7 +975,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$F$92:$F$96</c:f>
+              <c:f>Journal!$G$85:$G$89</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -966,7 +995,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$G$92:$G$96</c:f>
+              <c:f>Journal!$H$85:$H$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -980,7 +1009,7 @@
                   <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.75</c:v>
+                  <c:v>25.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,7 +1103,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
@@ -1658,16 +1687,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>178332</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257736</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>66272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>168807</xdr:rowOff>
+      <xdr:colOff>1590116</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>56747</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1692,13 +1721,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43607.504068518516" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="73">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43608.384906597224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="75">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-23T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-24T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1722,8 +1751,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="Type">
-  <location ref="F91:G96" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="G84:H89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1842,14 +1871,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E74">
-  <autoFilter ref="A1:E74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E76" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E76"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="1"/>
-    <tableColumn id="2" name="Temps (h)"/>
-    <tableColumn id="3" name="Type"/>
-    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="0"/>
-    <tableColumn id="5" name="Retour d'expérience"/>
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
+    <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
+    <tableColumn id="3" name="Type" dataDxfId="2"/>
+    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="5" name="Retour d'expérience" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2118,40 +2147,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScale="70" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2225,7 +2254,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="60">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="45">
       <c r="A7" s="6">
         <v>43592</v>
       </c>
@@ -2487,7 +2516,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A25" s="6">
         <v>43595</v>
       </c>
@@ -2594,7 +2623,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A32" s="6">
         <v>43599</v>
       </c>
@@ -2608,7 +2637,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A33" s="6">
         <v>43599</v>
       </c>
@@ -2667,7 +2696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" ht="90">
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A37" s="6">
         <v>43599</v>
       </c>
@@ -2684,7 +2713,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="38" spans="1:5" s="1" customFormat="1">
       <c r="A38" s="6">
         <v>43599</v>
       </c>
@@ -2698,7 +2727,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A39" s="6">
         <v>43600</v>
       </c>
@@ -2729,7 +2758,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A41" s="6">
         <v>43600</v>
       </c>
@@ -2746,7 +2775,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="1" customFormat="1" ht="75">
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="90">
       <c r="A42" s="6">
         <v>43600</v>
       </c>
@@ -2763,7 +2792,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A43" s="6">
         <v>43601</v>
       </c>
@@ -2805,7 +2834,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="1" customFormat="1" ht="75">
+    <row r="46" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A46" s="6">
         <v>43601</v>
       </c>
@@ -2847,7 +2876,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="1" customFormat="1" ht="105">
+    <row r="49" spans="1:5" s="1" customFormat="1" ht="120">
       <c r="A49" s="6">
         <v>43601</v>
       </c>
@@ -2864,7 +2893,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="1" customFormat="1" ht="75">
+    <row r="50" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A50" s="6">
         <v>43601</v>
       </c>
@@ -2878,7 +2907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="51" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A51" s="6">
         <v>43602</v>
       </c>
@@ -2926,7 +2955,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A54" s="6">
         <v>43602</v>
       </c>
@@ -2954,7 +2983,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="1" customFormat="1" ht="75">
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A56" s="6">
         <v>43602</v>
       </c>
@@ -2968,7 +2997,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A57" s="6">
         <v>43602</v>
       </c>
@@ -3013,7 +3042,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="60" spans="1:5" s="1" customFormat="1">
       <c r="A60" s="6">
         <v>43606</v>
       </c>
@@ -3027,7 +3056,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="61" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A61" s="6">
         <v>43606</v>
       </c>
@@ -3069,7 +3098,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="64" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A64" s="6">
         <v>43606</v>
       </c>
@@ -3083,7 +3112,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="1" customFormat="1" ht="60">
+    <row r="65" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A65" s="6">
         <v>43607</v>
       </c>
@@ -3125,10 +3154,10 @@
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="1" customFormat="1" ht="45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A68" s="6">
         <v>43607</v>
       </c>
@@ -3139,7 +3168,7 @@
         <v>6</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3156,17 +3185,47 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="1" customFormat="1">
-      <c r="A70" s="6"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" s="1" customFormat="1">
-      <c r="A71" s="6"/>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" s="1" customFormat="1">
-      <c r="A72" s="6"/>
-      <c r="D72" s="2"/>
+    <row r="70" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A70" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A71" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A72" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="73" spans="1:5" s="1" customFormat="1">
       <c r="A73" s="6"/>
@@ -3176,52 +3235,60 @@
       <c r="A74" s="6"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="91" spans="6:7">
-      <c r="F91" s="3" t="s">
+    <row r="75" spans="1:5" s="1" customFormat="1">
+      <c r="A75" s="6"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:5" s="1" customFormat="1">
+      <c r="A76" s="6"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="84" spans="7:8">
+      <c r="G84" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H84" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="6:7">
-      <c r="F92" s="4" t="s">
+    <row r="85" spans="7:8">
+      <c r="G85" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G92" s="5">
+      <c r="H85" s="5">
         <v>5.75</v>
       </c>
     </row>
-    <row r="93" spans="6:7">
-      <c r="F93" s="4" t="s">
+    <row r="86" spans="7:8">
+      <c r="G86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G93" s="5">
+      <c r="H86" s="5">
         <v>15.5</v>
       </c>
     </row>
-    <row r="94" spans="6:7">
-      <c r="F94" s="4" t="s">
+    <row r="87" spans="7:8">
+      <c r="G87" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G94" s="5">
+      <c r="H87" s="5">
         <v>10.75</v>
       </c>
     </row>
-    <row r="95" spans="6:7">
-      <c r="F95" s="4" t="s">
+    <row r="88" spans="7:8">
+      <c r="G88" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G95" s="5">
-        <v>23.75</v>
-      </c>
-    </row>
-    <row r="96" spans="6:7">
-      <c r="F96" s="4" t="s">
+      <c r="H88" s="5">
+        <v>25.25</v>
+      </c>
+    </row>
+    <row r="89" spans="7:8">
+      <c r="G89" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G96" s="5">
-        <v>55.75</v>
+      <c r="H89" s="5">
+        <v>57.25</v>
       </c>
     </row>
   </sheetData>
@@ -3231,7 +3298,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Gras"&amp;12Journal de travail&amp;C&amp;"-,Gras"&amp;14Runscape&amp;R&amp;"-,Gras"&amp;12TPI</oddHeader>
     <oddFooter>&amp;LPHILIBERT Alexandre&amp;CPage &amp;P&amp;R le &amp;D</oddFooter>

</xml_diff>

<commit_message>
Create new Wireframes for improved activityCreation page, Modified activityCreation page to correspond to wireframe
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
   <si>
     <t>Date</t>
   </si>
@@ -321,6 +321,30 @@
   </si>
   <si>
     <t>Création d'un test sur le endpoint des positions d'une activité</t>
+  </si>
+  <si>
+    <t>J'ai rencontré un problème ou les positions n'étaient pas dans l'ordre du timestamp, je n'ai pas tout de suite remarqué ce problème car je n'avais pas de comparaison avec d'autres résultats</t>
+  </si>
+  <si>
+    <t>Analyse de l'ajout de statistiques sur la page de visualisation d'une activité</t>
+  </si>
+  <si>
+    <t>Modification du wireframe, j'ajoute une section de statistiques. Je documente une solution pour ne plus avoir à effectuer la requête sur la ressource activity si celle-ci à déjà été effectuée auparavant</t>
+  </si>
+  <si>
+    <t>Ajout de la section de statistiques selon le wireframe.</t>
+  </si>
+  <si>
+    <t>Mise à jour de Trello</t>
+  </si>
+  <si>
+    <t>Création des wireframes de la page de création d'acitivité</t>
+  </si>
+  <si>
+    <t>Je m'appuie sur les idées fournis par Monsieur Glassey et Monsieur Lagona pour l'expérience utilisateur</t>
+  </si>
+  <si>
+    <t>Création de la nouvelle interface permettant la création d'activité</t>
   </si>
 </sst>
 </file>
@@ -827,7 +851,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$H$84</c:f>
+              <c:f>Journal!$H$88</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -975,7 +999,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$G$85:$G$89</c:f>
+              <c:f>Journal!$G$89:$G$93</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -995,21 +1019,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$H$85:$H$89</c:f>
+              <c:f>Journal!$H$89:$H$93</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.75</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.5</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.75</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.25</c:v>
+                  <c:v>26.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1689,13 +1713,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>66272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1590116</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>56747</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1721,16 +1745,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43608.384906597224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="75">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43608.610946064815" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="76">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-24T00:00:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-05-07T00:00:00" maxDate="2019-05-24T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.25" maxValue="2"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1738,7 +1762,7 @@
         <s v="Analyse"/>
         <s v="Conception"/>
         <s v="Implémentation"/>
-        <m/>
+        <m u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1751,8 +1775,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="G84:H89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="G88:H93" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1762,7 +1786,7 @@
         <item x="2"/>
         <item x="0"/>
         <item x="3"/>
-        <item h="1" x="4"/>
+        <item h="1" m="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1871,8 +1895,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E76" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E80" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E80"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2147,10 +2171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3185,7 +3209,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="70" spans="1:5" s="1" customFormat="1" ht="90">
       <c r="A70" s="6">
         <v>43608</v>
       </c>
@@ -3197,6 +3221,9 @@
       </c>
       <c r="D70" s="2" t="s">
         <v>94</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3227,68 +3254,147 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="1" customFormat="1">
-      <c r="A73" s="6"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" s="1" customFormat="1">
-      <c r="A74" s="6"/>
-      <c r="D74" s="2"/>
+    <row r="73" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A73" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A74" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B74" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="75" spans="1:5" s="1" customFormat="1">
-      <c r="A75" s="6"/>
-      <c r="D75" s="2"/>
+      <c r="A75" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="76" spans="1:5" s="1" customFormat="1">
-      <c r="A76" s="6"/>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="84" spans="7:8">
-      <c r="G84" s="3" t="s">
+      <c r="A76" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A77" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B77" s="1">
         <v>1</v>
       </c>
-      <c r="H84" t="s">
+      <c r="C77" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A78" s="6">
+        <v>43608</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="1" customFormat="1">
+      <c r="A79" s="6"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:5" s="1" customFormat="1">
+      <c r="A80" s="6"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="88" spans="7:8">
+      <c r="G88" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="7:8">
-      <c r="G85" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H85" s="5">
-        <v>5.75</v>
-      </c>
-    </row>
-    <row r="86" spans="7:8">
-      <c r="G86" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H86" s="5">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="87" spans="7:8">
-      <c r="G87" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H87" s="5">
-        <v>10.75</v>
-      </c>
-    </row>
-    <row r="88" spans="7:8">
-      <c r="G88" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H88" s="5">
-        <v>25.25</v>
       </c>
     </row>
     <row r="89" spans="7:8">
       <c r="G89" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H89" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="7:8">
+      <c r="G90" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H90" s="5">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="91" spans="7:8">
+      <c r="G91" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H91" s="5">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="92" spans="7:8">
+      <c r="G92" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H92" s="5">
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="93" spans="7:8">
+      <c r="G93" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H89" s="5">
-        <v>57.25</v>
+      <c r="H93" s="5">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new ActivityCreation Page is now finished, fixed background displacement when loading a page with scrollbar
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId2"/>
+    <pivotCache cacheId="3" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>Création de la nouvelle interface permettant la création d'activité</t>
+  </si>
+  <si>
+    <t>Correction d'un bug d'affichage. Lors du changement de page l'image de fond était déplacée si une barre de scroll apparaissait. J'ai changé le conteneur de scroll pour que ce ne soit pas le body de la page mais le conteneur d'une page qui scrollait</t>
+  </si>
+  <si>
+    <t>Correction d'un bug dans le header ou la page actuelle n'était pas sélectionnée lorsque la page était rechargée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation du refactoring de la page de création d'activité, j'y ajoute une barre de chargement pour l'upload des fichiers </t>
+  </si>
+  <si>
+    <t>Tests de la nouvelle page de création d'activité</t>
+  </si>
+  <si>
+    <t>Deploiement de la nouvelle interface sur AWS</t>
   </si>
 </sst>
 </file>
@@ -851,7 +866,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$H$88</c:f>
+              <c:f>Journal!$H$91</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -999,7 +1014,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$G$89:$G$93</c:f>
+              <c:f>Journal!$G$92:$G$96</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1019,7 +1034,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$H$89:$H$93</c:f>
+              <c:f>Journal!$H$92:$H$96</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1033,7 +1048,7 @@
                   <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.25</c:v>
+                  <c:v>29.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1713,13 +1728,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>66272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1590116</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>56747</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1745,16 +1760,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43608.610946064815" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="76">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43609.440322685186" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="81">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
-    <cacheField name="Date" numFmtId="164">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-05-07T00:00:00" maxDate="2019-05-24T00:00:00"/>
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-25T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.25" maxValue="2"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1762,7 +1777,7 @@
         <s v="Analyse"/>
         <s v="Conception"/>
         <s v="Implémentation"/>
-        <m u="1"/>
+        <m/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1775,8 +1790,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="G88:H93" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="G91:H96" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1786,7 +1801,7 @@
         <item x="2"/>
         <item x="0"/>
         <item x="3"/>
-        <item h="1" m="1" x="4"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1895,8 +1910,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E80" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E80"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E83" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E83"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2171,10 +2186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3341,60 +3356,122 @@
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="1" customFormat="1">
-      <c r="A79" s="6"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:5" s="1" customFormat="1">
-      <c r="A80" s="6"/>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="88" spans="7:8">
-      <c r="G88" s="3" t="s">
+    <row r="79" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A79" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B79" s="1">
         <v>1</v>
       </c>
-      <c r="H88" t="s">
+      <c r="C79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="1" customFormat="1" ht="75">
+      <c r="A80" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="1" customFormat="1" ht="30">
+      <c r="A81" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B81" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="1" customFormat="1">
+      <c r="A82" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="1" customFormat="1">
+      <c r="A83" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="G91" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H91" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="7:8">
-      <c r="G89" s="4" t="s">
+    <row r="92" spans="1:8">
+      <c r="G92" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H89" s="5">
+      <c r="H92" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="7:8">
-      <c r="G90" s="4" t="s">
+    <row r="93" spans="1:8">
+      <c r="G93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H90" s="5">
+      <c r="H93" s="5">
         <v>17.5</v>
       </c>
     </row>
-    <row r="91" spans="7:8">
-      <c r="G91" s="4" t="s">
+    <row r="94" spans="1:8">
+      <c r="G94" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H91" s="5">
+      <c r="H94" s="5">
         <v>11.25</v>
       </c>
     </row>
-    <row r="92" spans="7:8">
-      <c r="G92" s="4" t="s">
+    <row r="95" spans="1:8">
+      <c r="G95" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H92" s="5">
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="93" spans="7:8">
-      <c r="G93" s="4" t="s">
+      <c r="H95" s="5">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="G96" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H93" s="5">
-        <v>61</v>
+      <c r="H96" s="5">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transition on loadingBar width
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>Deploiement de la nouvelle interface sur AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise à jour des issues sur GitHub selon l'état actuel de l'application. J'ai également ouvert une nouvelle issue en lien avec </t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$H$91</c:f>
+              <c:f>Journal!$H$92</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1014,7 +1017,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$G$92:$G$96</c:f>
+              <c:f>Journal!$G$93:$G$97</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1034,7 +1037,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$H$92:$H$96</c:f>
+              <c:f>Journal!$H$93:$H$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1728,13 +1731,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>66272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1590116</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>56747</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1790,8 +1793,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="G91:H96" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="G92:H97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1910,8 +1913,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E83" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E84" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E84"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2186,10 +2189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I80" sqref="I80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3426,51 +3429,65 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
-      <c r="G91" s="3" t="s">
+    <row r="84" spans="1:8" s="1" customFormat="1" ht="45">
+      <c r="A84" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B84" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="G92" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H91" t="s">
+      <c r="H92" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="G92" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H92" s="5">
-        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:8">
       <c r="G93" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H93" s="5">
-        <v>17.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="G94" s="4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H94" s="5">
-        <v>11.25</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="G95" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H95" s="5">
-        <v>29.25</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="G96" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H96" s="5">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="97" spans="7:8">
+      <c r="G97" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H96" s="5">
+      <c r="H97" s="5">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a bug where the average speed without GPX was not being sent to the API
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mise à jour des issues sur GitHub selon l'état actuel de l'application. J'ai également ouvert une nouvelle issue en lien avec </t>
+  </si>
+  <si>
+    <t>Documentation des améliorations possibles pour la création d'activité .Mise à jour des uses cases de la création d'activité</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$H$92</c:f>
+              <c:f>Journal!$H$93</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1017,7 +1020,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$G$93:$G$97</c:f>
+              <c:f>Journal!$G$94:$G$98</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1037,7 +1040,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$H$93:$H$97</c:f>
+              <c:f>Journal!$H$94:$H$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1045,13 +1048,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.5</c:v>
+                  <c:v>17.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.25</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.25</c:v>
+                  <c:v>29.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1731,13 +1734,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>66272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1590116</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>56747</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1763,16 +1766,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43609.440322685186" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="81">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43609.508926273149" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="84">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
-    <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-25T00:00:00"/>
+    <cacheField name="Date" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-05-07T00:00:00" maxDate="2019-05-25T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.25" maxValue="2"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1780,7 +1783,7 @@
         <s v="Analyse"/>
         <s v="Conception"/>
         <s v="Implémentation"/>
-        <m/>
+        <m u="1"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1793,8 +1796,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="G92:H97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="G93:H98" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1804,7 +1807,7 @@
         <item x="2"/>
         <item x="0"/>
         <item x="3"/>
-        <item h="1" x="4"/>
+        <item h="1" m="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1913,8 +1916,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E84" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E85" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E85"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2189,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+      <selection activeCell="B79" sqref="B79:B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3443,52 +3446,66 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
-      <c r="G92" s="3" t="s">
+    <row r="85" spans="1:8" s="1" customFormat="1" ht="45">
+      <c r="A85" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B85" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="G93" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H92" t="s">
+      <c r="H93" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="G93" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H93" s="5">
-        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:8">
       <c r="G94" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H94" s="5">
-        <v>17.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:8">
       <c r="G95" s="4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H95" s="5">
-        <v>11.25</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="G96" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H96" s="5">
-        <v>29.25</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="97" spans="7:8">
       <c r="G97" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="5">
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="98" spans="7:8">
+      <c r="G98" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H97" s="5">
-        <v>64</v>
+      <c r="H98" s="5">
+        <v>66.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added image in activity table for activity visualization, Added multithreading support
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$69</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A:$E</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -365,7 +366,34 @@
     <t xml:space="preserve">Mise à jour des issues sur GitHub selon l'état actuel de l'application. J'ai également ouvert une nouvelle issue en lien avec </t>
   </si>
   <si>
-    <t>Documentation des améliorations possibles pour la création d'activité .Mise à jour des uses cases de la création d'activité</t>
+    <t>Test de l'interface de création d'activité sur AWS, je découvre un bug lors de la création d'activité sans GPX, le champs de la vitesse totale n'est pas calculé. Je le corrige en local mais je ne mets pas à jour AWS.</t>
+  </si>
+  <si>
+    <t>Mise à jour de la documentation de la méthodologie de test dans le rapport de travail. J'y ajoute les navigateurs sur lesquels j'entreprend mes tests. Je retravail la mise en page de la documentation</t>
+  </si>
+  <si>
+    <t>Documentation des améliorations possibles pour la création d'activité. Mise à jour des uses cases de la création d'activité</t>
+  </si>
+  <si>
+    <t>Je continue la documentation des améliorations possibles. Je parle des améliorations possibles du routeur sur le client web ainsi que des améliorations pour l'envoi des ressources liées sur l'API</t>
+  </si>
+  <si>
+    <t>Conception de l'ajout du multithreading sur l'application.</t>
+  </si>
+  <si>
+    <t>Ajout du multithreading dans l'application au niveau de la création du listener http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise à jour du Trello, ajout de nouvelle tâches </t>
+  </si>
+  <si>
+    <t>Tests de la nouvelle fonctionnalité de multithreading, j'installe Jmeter pour essayer d'effectuer un test de charge en local sur ma machine.</t>
+  </si>
+  <si>
+    <t>Mise à jour de la stratégie de test</t>
+  </si>
+  <si>
+    <t>Je voudrais effectuer des tests de charge après l'implémentation du multithreading sur l'application</t>
   </si>
 </sst>
 </file>
@@ -872,7 +900,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$H$93</c:f>
+              <c:f>Journal!$J$112</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1020,7 +1048,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$G$94:$G$98</c:f>
+              <c:f>Journal!$I$113:$I$117</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1040,7 +1068,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$H$94:$H$98</c:f>
+              <c:f>Journal!$J$113:$J$117</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1048,13 +1076,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.75</c:v>
+                  <c:v>21.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.75</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.75</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,15 +1761,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>257736</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>66272</xdr:rowOff>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>155920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1590116</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>56747</xdr:rowOff>
+      <xdr:colOff>1623733</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>146395</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1766,16 +1794,16 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43609.508926273149" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="84">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43613.473890740737" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="93">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-05-07T00:00:00" maxDate="2019-05-25T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-29T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.25" maxValue="2"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1783,7 +1811,7 @@
         <s v="Analyse"/>
         <s v="Conception"/>
         <s v="Implémentation"/>
-        <m u="1"/>
+        <m/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1796,8 +1824,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="G93:H98" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="I112:J117" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1807,7 +1835,7 @@
         <item x="2"/>
         <item x="0"/>
         <item x="3"/>
-        <item h="1" m="1" x="4"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1916,8 +1944,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E85" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E94" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E94"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2192,22 +2220,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79:B85"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
   </cols>
@@ -2369,7 +2398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="12" spans="1:8" s="1" customFormat="1">
       <c r="A12" s="6">
         <v>43592</v>
       </c>
@@ -2789,7 +2818,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="40" spans="1:5" s="1" customFormat="1">
       <c r="A40" s="6">
         <v>43600</v>
       </c>
@@ -2820,7 +2849,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="1" customFormat="1" ht="90">
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A42" s="6">
         <v>43600</v>
       </c>
@@ -2921,7 +2950,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="1" customFormat="1" ht="120">
+    <row r="49" spans="1:5" s="1" customFormat="1" ht="105">
       <c r="A49" s="6">
         <v>43601</v>
       </c>
@@ -3129,7 +3158,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="63" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A63" s="6">
         <v>43606</v>
       </c>
@@ -3157,7 +3186,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="1" customFormat="1" ht="75">
+    <row r="65" spans="1:5" s="1" customFormat="1" ht="60">
       <c r="A65" s="6">
         <v>43607</v>
       </c>
@@ -3188,7 +3217,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="67" spans="1:5" s="1" customFormat="1">
       <c r="A67" s="6">
         <v>43607</v>
       </c>
@@ -3230,7 +3259,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="1" customFormat="1" ht="90">
+    <row r="70" spans="1:5" s="1" customFormat="1" ht="75">
       <c r="A70" s="6">
         <v>43608</v>
       </c>
@@ -3261,7 +3290,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="72" spans="1:5" s="1" customFormat="1">
       <c r="A72" s="6">
         <v>43608</v>
       </c>
@@ -3362,7 +3391,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="1" customFormat="1" ht="45">
+    <row r="79" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A79" s="6">
         <v>43609</v>
       </c>
@@ -3390,7 +3419,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="81" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A81" s="6">
         <v>43609</v>
       </c>
@@ -3404,7 +3433,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="1" customFormat="1">
+    <row r="82" spans="1:5" s="1" customFormat="1">
       <c r="A82" s="6">
         <v>43609</v>
       </c>
@@ -3418,7 +3447,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="1" customFormat="1">
+    <row r="83" spans="1:5" s="1" customFormat="1">
       <c r="A83" s="6">
         <v>43609</v>
       </c>
@@ -3432,7 +3461,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="1" customFormat="1" ht="45">
+    <row r="84" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A84" s="6">
         <v>43609</v>
       </c>
@@ -3446,7 +3475,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="1" customFormat="1" ht="45">
+    <row r="85" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A85" s="6">
         <v>43609</v>
       </c>
@@ -3457,55 +3486,174 @@
         <v>20</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A86" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B86" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="G93" s="3" t="s">
+    <row r="87" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A87" s="6">
+        <v>43609</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A88" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B88" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="1" customFormat="1">
+      <c r="A89" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A90" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B90" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A91" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B91" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A92" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B92" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="1" customFormat="1">
+      <c r="A93" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B93" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="1" customFormat="1">
+      <c r="A94" s="6"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="112" spans="9:10">
+      <c r="I112" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H93" t="s">
+      <c r="J112" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
-      <c r="G94" s="4" t="s">
+    <row r="113" spans="9:10">
+      <c r="I113" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H94" s="5">
+      <c r="J113" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
-      <c r="G95" s="4" t="s">
+    <row r="114" spans="9:10">
+      <c r="I114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H95" s="5">
-        <v>17.75</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="G96" s="4" t="s">
+      <c r="J114" s="5">
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="115" spans="9:10">
+      <c r="I115" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H96" s="5">
-        <v>12.75</v>
-      </c>
-    </row>
-    <row r="97" spans="7:8">
-      <c r="G97" s="4" t="s">
+      <c r="J115" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="9:10">
+      <c r="I116" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H97" s="5">
-        <v>29.75</v>
-      </c>
-    </row>
-    <row r="98" spans="7:8">
-      <c r="G98" s="4" t="s">
+      <c r="J116" s="5">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="117" spans="9:10">
+      <c r="I117" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H98" s="5">
-        <v>66.25</v>
+      <c r="J117" s="5">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3514,7 +3662,7 @@
       <formula1>"Gestion, Analyse, Conception, Implémentation, "</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Gras"&amp;12Journal de travail&amp;C&amp;"-,Gras"&amp;14Runscape&amp;R&amp;"-,Gras"&amp;12TPI</oddHeader>

</xml_diff>

<commit_message>
Started pages unloading in router
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="123">
   <si>
     <t>Date</t>
   </si>
@@ -394,6 +394,12 @@
   </si>
   <si>
     <t>Je voudrais effectuer des tests de charge après l'implémentation du multithreading sur l'application</t>
+  </si>
+  <si>
+    <t>Analyse de l'ajout de rafraichissement de la page d'activité lorsque le sportif créer une nouvelle activité</t>
+  </si>
+  <si>
+    <t>Conception des modifications à apporter pour permettre de rafraichir la page</t>
   </si>
 </sst>
 </file>
@@ -900,7 +906,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$J$112</c:f>
+              <c:f>Journal!$J$115</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1048,7 +1054,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$I$113:$I$117</c:f>
+              <c:f>Journal!$I$116:$I$120</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1068,7 +1074,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$J$113:$J$117</c:f>
+              <c:f>Journal!$J$116:$J$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1762,13 +1768,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>235324</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>155920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1623733</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>146395</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1824,8 +1830,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="I112:J117" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="I115:J120" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1944,8 +1950,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E94" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E97" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E97"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2220,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J117"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I125" sqref="I125"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3604,55 +3610,87 @@
         <v>117</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="1" customFormat="1">
-      <c r="A94" s="6"/>
-      <c r="D94" s="2"/>
-    </row>
-    <row r="112" spans="9:10">
-      <c r="I112" s="3" t="s">
+    <row r="94" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A94" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A95" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="1" customFormat="1">
+      <c r="A96" s="6"/>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" s="1" customFormat="1">
+      <c r="A97" s="6"/>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="115" spans="9:10">
+      <c r="I115" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J112" t="s">
+      <c r="J115" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="113" spans="9:10">
-      <c r="I113" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J113" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="114" spans="9:10">
-      <c r="I114" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J114" s="5">
-        <v>21.75</v>
-      </c>
-    </row>
-    <row r="115" spans="9:10">
-      <c r="I115" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J115" s="5">
-        <v>13</v>
       </c>
     </row>
     <row r="116" spans="9:10">
       <c r="I116" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J116" s="5">
         <v>6</v>
-      </c>
-      <c r="J116" s="5">
-        <v>31.25</v>
       </c>
     </row>
     <row r="117" spans="9:10">
       <c r="I117" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J117" s="5">
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="118" spans="9:10">
+      <c r="I118" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="9:10">
+      <c r="I119" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J119" s="5">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="120" spans="9:10">
+      <c r="I120" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J117" s="5">
+      <c r="J120" s="5">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Journal and Rapport, Fixed an issue with website background where zooming out would cause background to repeat
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="6" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -387,9 +387,6 @@
     <t xml:space="preserve">Mise à jour du Trello, ajout de nouvelle tâches </t>
   </si>
   <si>
-    <t>Tests de la nouvelle fonctionnalité de multithreading, j'installe Jmeter pour essayer d'effectuer un test de charge en local sur ma machine.</t>
-  </si>
-  <si>
     <t>Mise à jour de la stratégie de test</t>
   </si>
   <si>
@@ -400,6 +397,15 @@
   </si>
   <si>
     <t>Conception des modifications à apporter pour permettre de rafraichir la page</t>
+  </si>
+  <si>
+    <t>Meeting hebdomadaire avec Monsieur Glassey.</t>
+  </si>
+  <si>
+    <t>Tests de la nouvelle fonctionnalité de multithreading, j'installe JMeter pour essayer d'effectuer un test de charge en local sur ma machine.</t>
+  </si>
+  <si>
+    <t>Ajout de la méthode de rafraichissement de la page des activités lorsqu'une nouvelle activité est insérée.</t>
   </si>
 </sst>
 </file>
@@ -906,7 +912,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$J$115</c:f>
+              <c:f>Journal!$J$120</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1054,7 +1060,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$I$116:$I$120</c:f>
+              <c:f>Journal!$I$121:$I$125</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1074,21 +1080,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$J$116:$J$120</c:f>
+              <c:f>Journal!$J$121:$J$125</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.75</c:v>
+                  <c:v>22.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.25</c:v>
+                  <c:v>32.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,13 +1774,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>235324</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>155920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1623733</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>146395</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1800,7 +1806,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43613.473890740737" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="93">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43613.698498958336" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="101">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
@@ -1830,8 +1836,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="I115:J120" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="I120:J125" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1950,8 +1956,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E97" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E97"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E102" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E102"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2226,10 +2232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3562,10 +3568,10 @@
         <v>20</v>
       </c>
       <c r="D90" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3593,7 +3599,7 @@
         <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1">
@@ -3621,7 +3627,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3635,63 +3641,103 @@
         <v>20</v>
       </c>
       <c r="D95" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="1" customFormat="1">
+      <c r="A96" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="1" customFormat="1">
-      <c r="A96" s="6"/>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="1:4" s="1" customFormat="1">
-      <c r="A97" s="6"/>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="115" spans="9:10">
-      <c r="I115" s="3" t="s">
+    <row r="97" spans="1:4" s="1" customFormat="1" ht="30">
+      <c r="A97" s="6">
+        <v>43613</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="1" customFormat="1">
+      <c r="A98" s="6"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" s="1" customFormat="1">
+      <c r="A99" s="6"/>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" s="1" customFormat="1">
+      <c r="A100" s="6"/>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" s="1" customFormat="1">
+      <c r="A101" s="6"/>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:4" s="1" customFormat="1">
+      <c r="A102" s="6"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="120" spans="9:10">
+      <c r="I120" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J115" t="s">
+      <c r="J120" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="9:10">
-      <c r="I116" s="4" t="s">
+    <row r="121" spans="9:10">
+      <c r="I121" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J116" s="5">
+      <c r="J121" s="5">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="122" spans="9:10">
+      <c r="I122" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J122" s="5">
+        <v>22.25</v>
+      </c>
+    </row>
+    <row r="123" spans="9:10">
+      <c r="I123" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J123" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="9:10">
+      <c r="I124" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="9:10">
-      <c r="I117" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J117" s="5">
-        <v>21.75</v>
-      </c>
-    </row>
-    <row r="118" spans="9:10">
-      <c r="I118" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J118" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="119" spans="9:10">
-      <c r="I119" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J119" s="5">
-        <v>31.25</v>
-      </c>
-    </row>
-    <row r="120" spans="9:10">
-      <c r="I120" s="4" t="s">
+      <c r="J124" s="5">
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="125" spans="9:10">
+      <c r="I125" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J120" s="5">
-        <v>72</v>
+      <c r="J125" s="5">
+        <v>75.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored dashboard interface with a new card system, Added new wireframe for new dashboard
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="128">
   <si>
     <t>Date</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>Ajout de la méthode de rafraichissement de la page des activités lorsqu'une nouvelle activité est insérée.</t>
+  </si>
+  <si>
+    <t>Création du nouveau wireframe pour la page d'affichage des activités</t>
+  </si>
+  <si>
+    <t>Je m'inspire du design proposé par TomTom MySports sur la page des statistiques</t>
+  </si>
+  <si>
+    <t>Implémentation de la nouvelle interface de dashboard des activités</t>
   </si>
 </sst>
 </file>
@@ -1836,7 +1845,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
   <location ref="I120:J125" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2234,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3658,7 +3667,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="1" customFormat="1" ht="30">
+    <row r="97" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A97" s="6">
         <v>43613</v>
       </c>
@@ -3672,23 +3681,46 @@
         <v>124</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="1" customFormat="1">
-      <c r="A98" s="6"/>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="1:4" s="1" customFormat="1">
-      <c r="A99" s="6"/>
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="1:4" s="1" customFormat="1">
+    <row r="98" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A98" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A99" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B99" s="1">
+        <v>1</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="1" customFormat="1">
       <c r="A100" s="6"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" s="1" customFormat="1">
+    <row r="101" spans="1:5" s="1" customFormat="1">
       <c r="A101" s="6"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" s="1" customFormat="1">
+    <row r="102" spans="1:5" s="1" customFormat="1">
       <c r="A102" s="6"/>
       <c r="D102" s="2"/>
     </row>

</xml_diff>

<commit_message>
Updated JournalDeBord and RapportDeTravail
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
   <si>
     <t>Date</t>
   </si>
@@ -415,6 +415,21 @@
   </si>
   <si>
     <t>Implémentation de la nouvelle interface de dashboard des activités</t>
+  </si>
+  <si>
+    <t>Mise àj our du wireframe en y ajoutant la date de début de l'activité</t>
+  </si>
+  <si>
+    <t>Ajout de la date de début</t>
+  </si>
+  <si>
+    <t>Push sur Github, Pull sur AWS, scan du cahier des charges et envoi à Monsieur Lagona</t>
+  </si>
+  <si>
+    <t>Relecture de la conception, correction de fautes d'orthographes</t>
+  </si>
+  <si>
+    <t>Relecture de l'analyse, correction des fautes d'orthographes et reformulation de certains paragraphes</t>
   </si>
 </sst>
 </file>
@@ -921,7 +936,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$J$120</c:f>
+              <c:f>Journal!$D$109</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1069,7 +1084,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$I$121:$I$125</c:f>
+              <c:f>Journal!$C$110:$C$114</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1089,21 +1104,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$J$121:$J$125</c:f>
+              <c:f>Journal!$D$110:$D$114</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.25</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.25</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.75</c:v>
+                  <c:v>34.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1782,15 +1797,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>235324</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>155920</xdr:rowOff>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1623733</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>146395</xdr:rowOff>
+      <xdr:colOff>459440</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>107174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1815,13 +1830,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43613.698498958336" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="101">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43614.502284837959" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="106">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-29T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-30T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1846,7 +1861,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="I120:J125" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="C109:D114" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1965,8 +1980,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E102" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E102"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E107" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
+  <autoFilter ref="A1:E107"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
@@ -2241,18 +2256,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A103" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111:E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -3703,7 +3718,7 @@
         <v>43614</v>
       </c>
       <c r="B99" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>6</v>
@@ -3712,64 +3727,134 @@
         <v>127</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="1" customFormat="1">
-      <c r="A100" s="6"/>
-      <c r="D100" s="2"/>
+    <row r="100" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A100" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="101" spans="1:5" s="1" customFormat="1">
-      <c r="A101" s="6"/>
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="1:5" s="1" customFormat="1">
-      <c r="A102" s="6"/>
-      <c r="D102" s="2"/>
-    </row>
-    <row r="120" spans="9:10">
-      <c r="I120" s="3" t="s">
+      <c r="A101" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A102" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A103" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A104" s="6">
+        <v>43614</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="1" customFormat="1">
+      <c r="A105" s="6"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:5" s="1" customFormat="1">
+      <c r="A106" s="6"/>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="1:5" s="1" customFormat="1">
+      <c r="A107" s="6"/>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="C109" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J120" t="s">
+      <c r="D109" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="9:10">
-      <c r="I121" s="4" t="s">
+    <row r="110" spans="1:5">
+      <c r="C110" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J121" s="5">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="122" spans="9:10">
-      <c r="I122" s="4" t="s">
+      <c r="D110" s="5">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="C111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J122" s="5">
-        <v>22.25</v>
-      </c>
-    </row>
-    <row r="123" spans="9:10">
-      <c r="I123" s="4" t="s">
+      <c r="D111" s="5">
+        <v>23.75</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="C112" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J123" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="124" spans="9:10">
-      <c r="I124" s="4" t="s">
+      <c r="D112" s="5">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4">
+      <c r="C113" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J124" s="5">
-        <v>32.75</v>
-      </c>
-    </row>
-    <row r="125" spans="9:10">
-      <c r="I125" s="4" t="s">
+      <c r="D113" s="5">
+        <v>34.25</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4">
+      <c r="C114" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J125" s="5">
-        <v>75.25</v>
+      <c r="D114" s="5">
+        <v>79.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added resume, modified activity creation to return only when positions where inserted in database
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="9" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="138">
   <si>
     <t>Date</t>
   </si>
@@ -417,9 +417,6 @@
     <t>Implémentation de la nouvelle interface de dashboard des activités</t>
   </si>
   <si>
-    <t>Mise àj our du wireframe en y ajoutant la date de début de l'activité</t>
-  </si>
-  <si>
     <t>Ajout de la date de début</t>
   </si>
   <si>
@@ -430,6 +427,24 @@
   </si>
   <si>
     <t>Relecture de l'analyse, correction des fautes d'orthographes et reformulation de certains paragraphes</t>
+  </si>
+  <si>
+    <t>Mise à jour du wireframe en y ajoutant la date de début de l'activité</t>
+  </si>
+  <si>
+    <t>Écriture du résumé du projet</t>
+  </si>
+  <si>
+    <t>Écriture du bilan personnel</t>
+  </si>
+  <si>
+    <t>Modification du diagramme de séquence de l'affichage de la page d'interprétation du parcours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des annexes au Rapport de Travail, explications des thermes techniques dans la documentation </t>
+  </si>
+  <si>
+    <t>Modification de la méthode d'insértion des positions dans le but d'optimiser la création d'activité</t>
   </si>
 </sst>
 </file>
@@ -473,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -485,7 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -496,9 +510,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="38">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -506,6 +598,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -936,7 +1040,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$D$109</c:f>
+              <c:f>Journal!$I$116</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1084,7 +1188,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$C$110:$C$114</c:f>
+              <c:f>Journal!$H$117:$H$121</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1104,7 +1208,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$D$110:$D$114</c:f>
+              <c:f>Journal!$I$117:$I$121</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1112,10 +1216,10 @@
                   <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.75</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.5</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>34.25</c:v>
@@ -1798,13 +1902,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>459440</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>107174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1830,13 +1934,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43614.502284837959" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="106">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43620.463622569441" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="110">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Date" numFmtId="164">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-05-30T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-06-05T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
@@ -1860,8 +1964,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="C109:D114" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="H116:I121" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1902,6 +2006,26 @@
   <dataFields count="1">
     <dataField name="Somme de Temps (h)" fld="1" baseField="0" baseItem="363412240"/>
   </dataFields>
+  <formats count="6">
+    <format dxfId="32">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
   <chartFormats count="6">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
@@ -1980,14 +2104,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E107" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <autoFilter ref="A1:E107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E111" headerRowDxfId="37" dataDxfId="36" totalsRowDxfId="35">
+  <autoFilter ref="A1:E111"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="4"/>
-    <tableColumn id="2" name="Temps (h)" dataDxfId="3"/>
-    <tableColumn id="3" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="1"/>
-    <tableColumn id="5" name="Retour d'expérience" dataDxfId="0"/>
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="34"/>
+    <tableColumn id="2" name="Temps (h)" dataDxfId="33"/>
+    <tableColumn id="3" name="Type" dataDxfId="29"/>
+    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="27"/>
+    <tableColumn id="5" name="Retour d'expérience" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2256,22 +2380,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A103" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111:E115"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="56.85546875" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="7" max="9" width="16.140625" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" customWidth="1"/>
@@ -2295,7 +2417,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>43592</v>
       </c>
       <c r="B2" s="1">
@@ -2309,7 +2431,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>43592</v>
       </c>
       <c r="B3" s="1">
@@ -2323,7 +2445,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>43592</v>
       </c>
       <c r="B4" s="1">
@@ -2337,7 +2459,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1" ht="30">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>43592</v>
       </c>
       <c r="B5" s="1">
@@ -2351,7 +2473,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>43592</v>
       </c>
       <c r="B6" s="1">
@@ -2365,7 +2487,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="45">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>43592</v>
       </c>
       <c r="B7" s="1">
@@ -2379,7 +2501,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>43592</v>
       </c>
       <c r="B8" s="1">
@@ -2392,8 +2514,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="6">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A9" s="5">
         <v>43592</v>
       </c>
       <c r="B9" s="1">
@@ -2407,7 +2529,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="30">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>43592</v>
       </c>
       <c r="B10" s="1">
@@ -2420,8 +2542,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="44.25" customHeight="1">
-      <c r="A11" s="6">
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A11" s="5">
         <v>43592</v>
       </c>
       <c r="B11" s="1">
@@ -2434,8 +2556,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1">
-      <c r="A12" s="6">
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A12" s="5">
         <v>43592</v>
       </c>
       <c r="B12" s="1">
@@ -2447,10 +2569,10 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>43593</v>
       </c>
       <c r="B13" s="1">
@@ -2464,7 +2586,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>43593</v>
       </c>
       <c r="B14" s="1">
@@ -2478,7 +2600,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="1" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>43593</v>
       </c>
       <c r="B15" s="1">
@@ -2492,7 +2614,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" s="1" customFormat="1" ht="63" customHeight="1">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>43593</v>
       </c>
       <c r="B16" s="1">
@@ -2509,7 +2631,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="105">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>43594</v>
       </c>
       <c r="B17" s="1">
@@ -2526,7 +2648,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>43594</v>
       </c>
       <c r="B18" s="1">
@@ -2540,7 +2662,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="75" customHeight="1">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>43594</v>
       </c>
       <c r="B19" s="1">
@@ -2554,7 +2676,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="65.25" customHeight="1">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>43594</v>
       </c>
       <c r="B20" s="1">
@@ -2568,7 +2690,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" ht="126.75" customHeight="1">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>43594</v>
       </c>
       <c r="B21" s="1">
@@ -2585,7 +2707,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" ht="83.25" customHeight="1">
-      <c r="A22" s="6">
+      <c r="A22" s="5">
         <v>43594</v>
       </c>
       <c r="B22" s="1">
@@ -2599,7 +2721,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A23" s="6">
+      <c r="A23" s="5">
         <v>43594</v>
       </c>
       <c r="B23" s="1">
@@ -2613,7 +2735,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A24" s="6">
+      <c r="A24" s="5">
         <v>43595</v>
       </c>
       <c r="B24" s="1">
@@ -2627,7 +2749,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A25" s="6">
+      <c r="A25" s="5">
         <v>43595</v>
       </c>
       <c r="B25" s="1">
@@ -2641,7 +2763,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" ht="126" customHeight="1">
-      <c r="A26" s="6">
+      <c r="A26" s="5">
         <v>43595</v>
       </c>
       <c r="B26" s="1">
@@ -2658,7 +2780,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A27" s="6">
+      <c r="A27" s="5">
         <v>43595</v>
       </c>
       <c r="B27" s="1">
@@ -2672,7 +2794,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A28" s="6">
+      <c r="A28" s="5">
         <v>43595</v>
       </c>
       <c r="B28" s="1">
@@ -2686,7 +2808,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" ht="92.25" customHeight="1">
-      <c r="A29" s="6">
+      <c r="A29" s="5">
         <v>43595</v>
       </c>
       <c r="B29" s="1">
@@ -2703,7 +2825,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A30" s="6">
+      <c r="A30" s="5">
         <v>43595</v>
       </c>
       <c r="B30" s="1">
@@ -2720,7 +2842,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>43595</v>
       </c>
       <c r="B31" s="1">
@@ -2734,7 +2856,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A32" s="6">
+      <c r="A32" s="5">
         <v>43599</v>
       </c>
       <c r="B32" s="1">
@@ -2748,7 +2870,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A33" s="6">
+      <c r="A33" s="5">
         <v>43599</v>
       </c>
       <c r="B33" s="1">
@@ -2762,7 +2884,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A34" s="6">
+      <c r="A34" s="5">
         <v>43599</v>
       </c>
       <c r="B34" s="1">
@@ -2779,7 +2901,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
-      <c r="A35" s="6">
+      <c r="A35" s="5">
         <v>43599</v>
       </c>
       <c r="B35" s="1">
@@ -2793,7 +2915,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
-      <c r="A36" s="6">
+      <c r="A36" s="5">
         <v>43599</v>
       </c>
       <c r="B36" s="1">
@@ -2807,7 +2929,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1" ht="75">
-      <c r="A37" s="6">
+      <c r="A37" s="5">
         <v>43599</v>
       </c>
       <c r="B37" s="1">
@@ -2824,7 +2946,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>43599</v>
       </c>
       <c r="B38" s="1">
@@ -2838,7 +2960,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A39" s="6">
+      <c r="A39" s="5">
         <v>43600</v>
       </c>
       <c r="B39" s="1">
@@ -2855,7 +2977,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1">
-      <c r="A40" s="6">
+      <c r="A40" s="5">
         <v>43600</v>
       </c>
       <c r="B40" s="1">
@@ -2869,7 +2991,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A41" s="6">
+      <c r="A41" s="5">
         <v>43600</v>
       </c>
       <c r="B41" s="1">
@@ -2886,7 +3008,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="75">
-      <c r="A42" s="6">
+      <c r="A42" s="5">
         <v>43600</v>
       </c>
       <c r="B42" s="1">
@@ -2903,7 +3025,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A43" s="6">
+      <c r="A43" s="5">
         <v>43601</v>
       </c>
       <c r="B43" s="1">
@@ -2917,7 +3039,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1">
-      <c r="A44" s="6">
+      <c r="A44" s="5">
         <v>43601</v>
       </c>
       <c r="B44" s="1">
@@ -2931,7 +3053,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A45" s="6">
+      <c r="A45" s="5">
         <v>43601</v>
       </c>
       <c r="B45" s="1">
@@ -2945,7 +3067,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A46" s="6">
+      <c r="A46" s="5">
         <v>43601</v>
       </c>
       <c r="B46" s="1">
@@ -2959,7 +3081,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A47" s="6">
+      <c r="A47" s="5">
         <v>43601</v>
       </c>
       <c r="B47" s="1">
@@ -2973,7 +3095,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1">
-      <c r="A48" s="6">
+      <c r="A48" s="5">
         <v>43601</v>
       </c>
       <c r="B48" s="1">
@@ -2987,7 +3109,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="105">
-      <c r="A49" s="6">
+      <c r="A49" s="5">
         <v>43601</v>
       </c>
       <c r="B49" s="1">
@@ -3004,7 +3126,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A50" s="6">
+      <c r="A50" s="5">
         <v>43601</v>
       </c>
       <c r="B50" s="1">
@@ -3018,7 +3140,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A51" s="6">
+      <c r="A51" s="5">
         <v>43602</v>
       </c>
       <c r="B51" s="1">
@@ -3032,7 +3154,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A52" s="6">
+      <c r="A52" s="5">
         <v>43602</v>
       </c>
       <c r="B52" s="1">
@@ -3049,7 +3171,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A53" s="6">
+      <c r="A53" s="5">
         <v>43602</v>
       </c>
       <c r="B53" s="1">
@@ -3066,7 +3188,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A54" s="6">
+      <c r="A54" s="5">
         <v>43602</v>
       </c>
       <c r="B54" s="1">
@@ -3080,7 +3202,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A55" s="6">
+      <c r="A55" s="5">
         <v>43602</v>
       </c>
       <c r="B55" s="1">
@@ -3094,7 +3216,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A56" s="6">
+      <c r="A56" s="5">
         <v>43602</v>
       </c>
       <c r="B56" s="1">
@@ -3108,7 +3230,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A57" s="6">
+      <c r="A57" s="5">
         <v>43602</v>
       </c>
       <c r="B57" s="1">
@@ -3122,7 +3244,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A58" s="6">
+      <c r="A58" s="5">
         <v>43606</v>
       </c>
       <c r="B58" s="1">
@@ -3139,7 +3261,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1">
-      <c r="A59" s="6">
+      <c r="A59" s="5">
         <v>43606</v>
       </c>
       <c r="B59" s="1">
@@ -3153,7 +3275,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1">
-      <c r="A60" s="6">
+      <c r="A60" s="5">
         <v>43606</v>
       </c>
       <c r="B60" s="1">
@@ -3167,7 +3289,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A61" s="6">
+      <c r="A61" s="5">
         <v>43606</v>
       </c>
       <c r="B61" s="1">
@@ -3181,7 +3303,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A62" s="6">
+      <c r="A62" s="5">
         <v>43606</v>
       </c>
       <c r="B62" s="1">
@@ -3195,7 +3317,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A63" s="6">
+      <c r="A63" s="5">
         <v>43606</v>
       </c>
       <c r="B63" s="1">
@@ -3209,7 +3331,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A64" s="6">
+      <c r="A64" s="5">
         <v>43606</v>
       </c>
       <c r="B64" s="1">
@@ -3223,7 +3345,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A65" s="6">
+      <c r="A65" s="5">
         <v>43607</v>
       </c>
       <c r="B65" s="1">
@@ -3240,7 +3362,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A66" s="6">
+      <c r="A66" s="5">
         <v>43607</v>
       </c>
       <c r="B66" s="1">
@@ -3254,7 +3376,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" s="1" customFormat="1">
-      <c r="A67" s="6">
+      <c r="A67" s="5">
         <v>43607</v>
       </c>
       <c r="B67" s="1">
@@ -3268,7 +3390,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A68" s="6">
+      <c r="A68" s="5">
         <v>43607</v>
       </c>
       <c r="B68" s="1">
@@ -3282,7 +3404,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A69" s="6">
+      <c r="A69" s="5">
         <v>43607</v>
       </c>
       <c r="B69" s="1">
@@ -3296,7 +3418,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" s="1" customFormat="1" ht="75">
-      <c r="A70" s="6">
+      <c r="A70" s="5">
         <v>43608</v>
       </c>
       <c r="B70" s="1">
@@ -3313,7 +3435,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A71" s="6">
+      <c r="A71" s="5">
         <v>43608</v>
       </c>
       <c r="B71" s="1">
@@ -3327,7 +3449,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="1" customFormat="1">
-      <c r="A72" s="6">
+      <c r="A72" s="5">
         <v>43608</v>
       </c>
       <c r="B72" s="1">
@@ -3341,7 +3463,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A73" s="6">
+      <c r="A73" s="5">
         <v>43608</v>
       </c>
       <c r="B73" s="1">
@@ -3355,7 +3477,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A74" s="6">
+      <c r="A74" s="5">
         <v>43608</v>
       </c>
       <c r="B74" s="1">
@@ -3369,7 +3491,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="1" customFormat="1">
-      <c r="A75" s="6">
+      <c r="A75" s="5">
         <v>43608</v>
       </c>
       <c r="B75" s="1">
@@ -3383,7 +3505,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" s="1" customFormat="1">
-      <c r="A76" s="6">
+      <c r="A76" s="5">
         <v>43608</v>
       </c>
       <c r="B76" s="1">
@@ -3397,7 +3519,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A77" s="6">
+      <c r="A77" s="5">
         <v>43608</v>
       </c>
       <c r="B77" s="1">
@@ -3414,7 +3536,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A78" s="6">
+      <c r="A78" s="5">
         <v>43608</v>
       </c>
       <c r="B78" s="1">
@@ -3428,7 +3550,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A79" s="6">
+      <c r="A79" s="5">
         <v>43609</v>
       </c>
       <c r="B79" s="1">
@@ -3442,7 +3564,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="1" customFormat="1" ht="75">
-      <c r="A80" s="6">
+      <c r="A80" s="5">
         <v>43609</v>
       </c>
       <c r="B80" s="1">
@@ -3456,7 +3578,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A81" s="6">
+      <c r="A81" s="5">
         <v>43609</v>
       </c>
       <c r="B81" s="1">
@@ -3470,7 +3592,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1">
-      <c r="A82" s="6">
+      <c r="A82" s="5">
         <v>43609</v>
       </c>
       <c r="B82" s="1">
@@ -3484,7 +3606,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1">
-      <c r="A83" s="6">
+      <c r="A83" s="5">
         <v>43609</v>
       </c>
       <c r="B83" s="1">
@@ -3498,7 +3620,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A84" s="6">
+      <c r="A84" s="5">
         <v>43609</v>
       </c>
       <c r="B84" s="1">
@@ -3512,7 +3634,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A85" s="6">
+      <c r="A85" s="5">
         <v>43609</v>
       </c>
       <c r="B85" s="1">
@@ -3526,7 +3648,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A86" s="6">
+      <c r="A86" s="5">
         <v>43609</v>
       </c>
       <c r="B86" s="1">
@@ -3540,7 +3662,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A87" s="6">
+      <c r="A87" s="5">
         <v>43609</v>
       </c>
       <c r="B87" s="1">
@@ -3554,7 +3676,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="60">
-      <c r="A88" s="6">
+      <c r="A88" s="5">
         <v>43613</v>
       </c>
       <c r="B88" s="1">
@@ -3568,7 +3690,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" s="1" customFormat="1">
-      <c r="A89" s="6">
+      <c r="A89" s="5">
         <v>43613</v>
       </c>
       <c r="B89" s="1">
@@ -3582,7 +3704,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A90" s="6">
+      <c r="A90" s="5">
         <v>43613</v>
       </c>
       <c r="B90" s="1">
@@ -3599,7 +3721,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A91" s="6">
+      <c r="A91" s="5">
         <v>43613</v>
       </c>
       <c r="B91" s="1">
@@ -3613,7 +3735,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A92" s="6">
+      <c r="A92" s="5">
         <v>43613</v>
       </c>
       <c r="B92" s="1">
@@ -3627,7 +3749,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1">
-      <c r="A93" s="6">
+      <c r="A93" s="5">
         <v>43613</v>
       </c>
       <c r="B93" s="1">
@@ -3641,7 +3763,7 @@
       </c>
     </row>
     <row r="94" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A94" s="6">
+      <c r="A94" s="5">
         <v>43613</v>
       </c>
       <c r="B94" s="1">
@@ -3655,7 +3777,7 @@
       </c>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A95" s="6">
+      <c r="A95" s="5">
         <v>43613</v>
       </c>
       <c r="B95" s="1">
@@ -3669,7 +3791,7 @@
       </c>
     </row>
     <row r="96" spans="1:5" s="1" customFormat="1">
-      <c r="A96" s="6">
+      <c r="A96" s="5">
         <v>43613</v>
       </c>
       <c r="B96" s="1">
@@ -3683,7 +3805,7 @@
       </c>
     </row>
     <row r="97" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A97" s="6">
+      <c r="A97" s="5">
         <v>43613</v>
       </c>
       <c r="B97" s="1">
@@ -3697,7 +3819,7 @@
       </c>
     </row>
     <row r="98" spans="1:5" s="1" customFormat="1" ht="45">
-      <c r="A98" s="6">
+      <c r="A98" s="5">
         <v>43614</v>
       </c>
       <c r="B98" s="1">
@@ -3714,7 +3836,7 @@
       </c>
     </row>
     <row r="99" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A99" s="6">
+      <c r="A99" s="5">
         <v>43614</v>
       </c>
       <c r="B99" s="1">
@@ -3728,7 +3850,7 @@
       </c>
     </row>
     <row r="100" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A100" s="6">
+      <c r="A100" s="5">
         <v>43614</v>
       </c>
       <c r="B100" s="1">
@@ -3738,11 +3860,11 @@
         <v>20</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="1" customFormat="1">
-      <c r="A101" s="6">
+      <c r="A101" s="5">
         <v>43614</v>
       </c>
       <c r="B101" s="1">
@@ -3752,11 +3874,11 @@
         <v>6</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A102" s="6">
+      <c r="A102" s="5">
         <v>43614</v>
       </c>
       <c r="B102" s="1">
@@ -3766,11 +3888,11 @@
         <v>4</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A103" s="6">
+      <c r="A103" s="5">
         <v>43614</v>
       </c>
       <c r="B103" s="1">
@@ -3780,11 +3902,11 @@
         <v>5</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="1" customFormat="1" ht="30">
-      <c r="A104" s="6">
+      <c r="A104" s="5">
         <v>43614</v>
       </c>
       <c r="B104" s="1">
@@ -3794,67 +3916,133 @@
         <v>20</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="1" customFormat="1">
-      <c r="A105" s="6"/>
-      <c r="D105" s="2"/>
+      <c r="A105" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="106" spans="1:5" s="1" customFormat="1">
-      <c r="A106" s="6"/>
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="1:5" s="1" customFormat="1">
-      <c r="A107" s="6"/>
-      <c r="D107" s="2"/>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="C109" s="3" t="s">
+      <c r="A106" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B106" s="1">
         <v>1</v>
       </c>
-      <c r="D109" t="s">
+      <c r="C106" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A107" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A108" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" s="1" customFormat="1" ht="30">
+      <c r="A109" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="1" customFormat="1">
+      <c r="A110" s="5"/>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:5" s="1" customFormat="1">
+      <c r="A111" s="5"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="116" spans="8:9" ht="30">
+      <c r="H116" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I116" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
-      <c r="C110" s="4" t="s">
+    <row r="117" spans="8:9">
+      <c r="H117" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D110" s="5">
+      <c r="I117" s="2">
         <v>6.75</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
-      <c r="C111" s="4" t="s">
+    <row r="118" spans="8:9">
+      <c r="H118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D111" s="5">
-        <v>23.75</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="C112" s="4" t="s">
+      <c r="I118" s="2">
+        <v>24.75</v>
+      </c>
+    </row>
+    <row r="119" spans="8:9">
+      <c r="H119" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D112" s="5">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="113" spans="3:4">
-      <c r="C113" s="4" t="s">
+      <c r="I119" s="2">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="120" spans="8:9">
+      <c r="H120" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D113" s="5">
+      <c r="I120" s="2">
         <v>34.25</v>
       </c>
     </row>
-    <row r="114" spans="3:4">
-      <c r="C114" s="4" t="s">
+    <row r="121" spans="8:9">
+      <c r="H121" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D114" s="5">
-        <v>79.25</v>
+      <c r="I121" s="2">
+        <v>83.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Docs, worked on resume, Changed behavior of activity creation to only respond when positions where inserted in database
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId2"/>
+    <pivotCache cacheId="3" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -132,9 +132,6 @@
     <t>Modification de la création d'activité dans le modèle d'activité pour prendre en compte les champs traité par le middleware Formidable. J'ai créer une méthode dans la classe d'utility pour me permettre de changer le nom des propriétés d'un objet, cela va m'être utile lorsque les paramètres d'une requête HTTP ne correspondent pas aux noms de champs dans la base de données</t>
   </si>
   <si>
-    <t>Je me suis rendu compte que les timestamps étaient décaler d'une heure, j'ai dabord cru que le problème vennait du format de timestmap que je fournissait en paramètre, mais le problème vennait en faite de la connection au serveur MySQL, je ne spécifait pas le timezone.</t>
-  </si>
-  <si>
     <t>Tests des modifications apportées sur le endpoint de création d'activités. J'effectue les tests avec des GPX fournit par Monsieur Glassey. Après ces tests je lance la liste complète des tests pour vérifier que je n'ai pas casser une autre fonctionnalité de l'API</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>Modification de la méthode d'insértion des positions dans le but d'optimiser la création d'activité</t>
+  </si>
+  <si>
+    <t>Je me suis rendu compte que les timestamps étaient décalé d'une heure, j'ai d'abord cru que le problème vennait du format de timestmap que je fournissais en paramètre, mais le problème vennait en faite de la connection au serveur MySQL, je ne spécifiais pas la timezone.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="20">
     <dxf>
       <alignment wrapText="0" readingOrder="0"/>
     </dxf>
@@ -530,13 +530,30 @@
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
@@ -555,77 +572,6 @@
     </dxf>
     <dxf>
       <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1216,13 +1162,13 @@
                   <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.75</c:v>
+                  <c:v>24.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.25</c:v>
+                  <c:v>34.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1934,7 +1880,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43620.463622569441" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="110">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43620.565448148147" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="110">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
@@ -1964,7 +1910,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
   <location ref="H116:I121" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -2007,22 +1953,22 @@
     <dataField name="Somme de Temps (h)" fld="1" baseField="0" baseItem="363412240"/>
   </dataFields>
   <formats count="6">
-    <format dxfId="32">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -2104,14 +2050,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E111" headerRowDxfId="37" dataDxfId="36" totalsRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E111" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
   <autoFilter ref="A1:E111"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="34"/>
-    <tableColumn id="2" name="Temps (h)" dataDxfId="33"/>
-    <tableColumn id="3" name="Type" dataDxfId="29"/>
-    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="27"/>
-    <tableColumn id="5" name="Retour d'expérience" dataDxfId="28"/>
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="10"/>
+    <tableColumn id="2" name="Temps (h)" dataDxfId="9"/>
+    <tableColumn id="3" name="Type" dataDxfId="8"/>
+    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="7"/>
+    <tableColumn id="5" name="Retour d'expérience" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2382,8 +2328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2703,7 +2649,7 @@
         <v>32</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" ht="83.25" customHeight="1">
@@ -2717,7 +2663,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1">
@@ -2731,7 +2677,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" ht="52.5" customHeight="1">
@@ -2745,7 +2691,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="30">
@@ -2759,7 +2705,7 @@
         <v>5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" ht="126" customHeight="1">
@@ -2773,10 +2719,10 @@
         <v>20</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" ht="59.25" customHeight="1">
@@ -2790,7 +2736,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" ht="49.5" customHeight="1">
@@ -2804,7 +2750,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" ht="92.25" customHeight="1">
@@ -2818,10 +2764,10 @@
         <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="1" customFormat="1" ht="60">
@@ -2835,10 +2781,10 @@
         <v>20</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" ht="30">
@@ -2852,7 +2798,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" ht="45">
@@ -2866,7 +2812,7 @@
         <v>20</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" ht="45">
@@ -2880,7 +2826,7 @@
         <v>20</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" ht="60">
@@ -2894,10 +2840,10 @@
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1">
@@ -2911,7 +2857,7 @@
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1">
@@ -2939,10 +2885,10 @@
         <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1">
@@ -2956,7 +2902,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" ht="60">
@@ -2970,10 +2916,10 @@
         <v>20</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1">
@@ -2987,7 +2933,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3001,10 +2947,10 @@
         <v>6</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="75">
@@ -3018,10 +2964,10 @@
         <v>6</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3035,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1">
@@ -3049,7 +2995,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3063,7 +3009,7 @@
         <v>20</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3077,7 +3023,7 @@
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3091,7 +3037,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1">
@@ -3105,7 +3051,7 @@
         <v>20</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="105">
@@ -3119,10 +3065,10 @@
         <v>20</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3136,7 +3082,7 @@
         <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3150,7 +3096,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3164,10 +3110,10 @@
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3181,10 +3127,10 @@
         <v>20</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3198,7 +3144,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3212,7 +3158,7 @@
         <v>20</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3226,7 +3172,7 @@
         <v>20</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3240,7 +3186,7 @@
         <v>20</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3254,10 +3200,10 @@
         <v>6</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1">
@@ -3271,7 +3217,7 @@
         <v>5</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1">
@@ -3285,7 +3231,7 @@
         <v>4</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3299,7 +3245,7 @@
         <v>6</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3313,7 +3259,7 @@
         <v>4</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3327,7 +3273,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3341,7 +3287,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3355,10 +3301,10 @@
         <v>20</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3372,7 +3318,7 @@
         <v>20</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="1" customFormat="1">
@@ -3386,7 +3332,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3400,7 +3346,7 @@
         <v>6</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3414,7 +3360,7 @@
         <v>6</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="1" customFormat="1" ht="75">
@@ -3428,10 +3374,10 @@
         <v>6</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3445,7 +3391,7 @@
         <v>6</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="1" customFormat="1">
@@ -3459,7 +3405,7 @@
         <v>20</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3473,7 +3419,7 @@
         <v>5</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3487,7 +3433,7 @@
         <v>20</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="1" customFormat="1">
@@ -3501,7 +3447,7 @@
         <v>6</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="1" customFormat="1">
@@ -3515,7 +3461,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3529,10 +3475,10 @@
         <v>20</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3546,7 +3492,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3560,7 +3506,7 @@
         <v>6</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="1" customFormat="1" ht="75">
@@ -3574,7 +3520,7 @@
         <v>6</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3588,7 +3534,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1">
@@ -3602,7 +3548,7 @@
         <v>6</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1">
@@ -3616,7 +3562,7 @@
         <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3630,7 +3576,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3644,7 +3590,7 @@
         <v>20</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3658,7 +3604,7 @@
         <v>6</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3672,7 +3618,7 @@
         <v>20</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3686,7 +3632,7 @@
         <v>20</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="1" customFormat="1">
@@ -3700,7 +3646,7 @@
         <v>20</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3714,10 +3660,10 @@
         <v>20</v>
       </c>
       <c r="D90" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E90" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3731,7 +3677,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3745,7 +3691,7 @@
         <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1">
@@ -3759,7 +3705,7 @@
         <v>4</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3773,7 +3719,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3787,7 +3733,7 @@
         <v>20</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="1" customFormat="1">
@@ -3801,7 +3747,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3815,7 +3761,7 @@
         <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3829,10 +3775,10 @@
         <v>20</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E98" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3846,7 +3792,7 @@
         <v>6</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3860,7 +3806,7 @@
         <v>20</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="1" customFormat="1">
@@ -3874,7 +3820,7 @@
         <v>6</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3888,7 +3834,7 @@
         <v>4</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3902,7 +3848,7 @@
         <v>5</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3916,7 +3862,7 @@
         <v>20</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="1" customFormat="1">
@@ -3930,7 +3876,7 @@
         <v>4</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="1" customFormat="1">
@@ -3944,7 +3890,7 @@
         <v>4</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3958,7 +3904,7 @@
         <v>20</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3972,7 +3918,7 @@
         <v>4</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3986,7 +3932,7 @@
         <v>6</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:5" s="1" customFormat="1">
@@ -4018,7 +3964,7 @@
         <v>20</v>
       </c>
       <c r="I118" s="2">
-        <v>24.75</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="119" spans="8:9">
@@ -4034,7 +3980,7 @@
         <v>6</v>
       </c>
       <c r="I120" s="2">
-        <v>34.25</v>
+        <v>34.75</v>
       </c>
     </row>
     <row r="121" spans="8:9">

</xml_diff>

<commit_message>
Updated README, added PlanificationFinale, Updated RapportDeTravail
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Il est possbile, sur firefox, d'envoyer une requête contenant des dates de début et de fin d'activité érronés. La requête est néanmoins stoppée sur le serveur lors de la validation du format de timestamp</t>
   </si>
   <si>
-    <t>Gestion des erreurs sur le client</t>
-  </si>
-  <si>
     <t>Correction d'un bug ou l'un des appels XHR ne s'effectuait pas aux chargement de la page (lieux)</t>
   </si>
   <si>
@@ -246,18 +243,12 @@
     <t>Corrections de bug dans le router du client web, à certains moment les pages n'étaient pas changées</t>
   </si>
   <si>
-    <t>Ajout du highlight de l'élément courant dans le menu de l'application</t>
-  </si>
-  <si>
     <t>J'ai dû modifier le header pour y ajouter une méthode permettant de notifier les items du menu lorsqu'un changement de page a lieu</t>
   </si>
   <si>
     <t>J'ai trouvé un site web qui mets en avant 3 possibilités pour améliorer les relations entre les ressources de l'API</t>
   </si>
   <si>
-    <t>Conception d'améliorations possibles pour les requêtes de selection d'activités. Je documente les différentes options qui sont disponible pour améliorer les relations entre les ressources</t>
-  </si>
-  <si>
     <t>Analyse des besoins du sportif pour la fonctionnalité de visualisation d'activités sous forme de carte</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
     <t>Modification du routeur du client web pour pouvoir passer des parmètres aux pages à charger</t>
   </si>
   <si>
-    <t>Je continue la cration de la page d'affichage d'une activité, j'ai écris une fonction utilisant le module node gps-distance pour calculer le pace par km du côté client</t>
-  </si>
-  <si>
     <t>Documentation de la fonction calculant le pace, j'avais des doutes sur le temps d'exécution de la fonction sachant que lors du calcul de certains parcours plus de 20'000 points devaient être calculés.</t>
   </si>
   <si>
@@ -327,18 +315,12 @@
     <t>Analyse de l'ajout de statistiques sur la page de visualisation d'une activité</t>
   </si>
   <si>
-    <t>Modification du wireframe, j'ajoute une section de statistiques. Je documente une solution pour ne plus avoir à effectuer la requête sur la ressource activity si celle-ci à déjà été effectuée auparavant</t>
-  </si>
-  <si>
     <t>Ajout de la section de statistiques selon le wireframe.</t>
   </si>
   <si>
     <t>Mise à jour de Trello</t>
   </si>
   <si>
-    <t>Création des wireframes de la page de création d'acitivité</t>
-  </si>
-  <si>
     <t>Je m'appuie sur les idées fournis par Monsieur Glassey et Monsieur Lagona pour l'expérience utilisateur</t>
   </si>
   <si>
@@ -441,10 +423,37 @@
     <t xml:space="preserve">Ajout des annexes au Rapport de Travail, explications des thermes techniques dans la documentation </t>
   </si>
   <si>
-    <t>Modification de la méthode d'insértion des positions dans le but d'optimiser la création d'activité</t>
-  </si>
-  <si>
     <t>Je me suis rendu compte que les timestamps étaient décalé d'une heure, j'ai d'abord cru que le problème vennait du format de timestmap que je fournissais en paramètre, mais le problème vennait en faite de la connection au serveur MySQL, je ne spécifiais pas la timezone.</t>
+  </si>
+  <si>
+    <t>Entretien hebdomadaire avec Monsieur Glassey. Nous avons discuté de l'approche que je pourrais avoir lors de la présentation du TPI (quels éléments pourraient être présenté etc..)</t>
+  </si>
+  <si>
+    <t>Les tests automatisé me permettent de facilement m'aperçevoir si j'ai cassé une partie de l'application</t>
+  </si>
+  <si>
+    <t>Gestion des erreurs sur le client (page création d'activité)</t>
+  </si>
+  <si>
+    <t>Ajout du highlight de l'élément courant dans le menu de l'application (activités, créer une activité)</t>
+  </si>
+  <si>
+    <t>Conception d'améliorations possibles pour les requêtes de sélection d'activités. Je documente les différentes options qui sont disponible pour améliorer les relations entre les ressources</t>
+  </si>
+  <si>
+    <t>Je continue la création de la page d'affichage d'une activité, j'ai écris une fonction utilisant le module node gps-distance pour calculer le pace par km du côté client</t>
+  </si>
+  <si>
+    <t>Modification du wireframe, j'ajoute une section de statistiques.</t>
+  </si>
+  <si>
+    <t>Création des wireframes de la page de création d'activité</t>
+  </si>
+  <si>
+    <t>Modification de la méthode d'insertion des positions dans le but d'optimiser la création d'activité</t>
+  </si>
+  <si>
+    <t>Création de la planification finale</t>
   </si>
 </sst>
 </file>
@@ -986,7 +995,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$I$116</c:f>
+              <c:f>Journal!$I$121</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1134,7 +1143,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$H$117:$H$121</c:f>
+              <c:f>Journal!$H$122:$H$126</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1154,7 +1163,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$I$117:$I$121</c:f>
+              <c:f>Journal!$I$122:$I$126</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1165,7 +1174,7 @@
                   <c:v>24.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.5</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>34.75</c:v>
@@ -1848,13 +1857,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>459440</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>107174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1880,7 +1889,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43620.565448148147" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="110">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43620.702379745373" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="115">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
@@ -1911,7 +1920,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="H116:I121" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="H121:I126" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -2050,8 +2059,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E111" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
-  <autoFilter ref="A1:E111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E116" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
+  <autoFilter ref="A1:E116"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="10"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="9"/>
@@ -2326,10 +2335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="E110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I124" sqref="I124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2649,7 +2658,7 @@
         <v>32</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" ht="83.25" customHeight="1">
@@ -2665,6 +2674,9 @@
       <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" ht="94.5" customHeight="1">
       <c r="A23" s="5">
@@ -2981,7 +2993,7 @@
         <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1">
@@ -2995,7 +3007,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3009,7 +3021,7 @@
         <v>20</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3023,7 +3035,7 @@
         <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3037,7 +3049,7 @@
         <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1">
@@ -3051,7 +3063,7 @@
         <v>20</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="105">
@@ -3065,10 +3077,10 @@
         <v>20</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3082,7 +3094,7 @@
         <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3096,7 +3108,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3110,10 +3122,10 @@
         <v>6</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3127,10 +3139,10 @@
         <v>20</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3144,7 +3156,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3158,7 +3170,7 @@
         <v>20</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3172,7 +3184,7 @@
         <v>20</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3186,7 +3198,7 @@
         <v>20</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3200,10 +3212,10 @@
         <v>6</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1">
@@ -3217,7 +3229,7 @@
         <v>5</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1">
@@ -3231,7 +3243,7 @@
         <v>4</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3245,7 +3257,7 @@
         <v>6</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3259,7 +3271,7 @@
         <v>4</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3273,7 +3285,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3287,7 +3299,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3301,10 +3313,10 @@
         <v>20</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3318,7 +3330,7 @@
         <v>20</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="1" customFormat="1">
@@ -3332,7 +3344,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3346,7 +3358,7 @@
         <v>6</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3360,7 +3372,7 @@
         <v>6</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="1" customFormat="1" ht="75">
@@ -3374,10 +3386,10 @@
         <v>6</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3391,10 +3403,10 @@
         <v>6</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="1" customFormat="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="1" customFormat="1" ht="35.25" customHeight="1">
       <c r="A72" s="5">
         <v>43608</v>
       </c>
@@ -3405,7 +3417,7 @@
         <v>20</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3419,10 +3431,10 @@
         <v>5</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="1" customFormat="1" ht="60">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="1" customFormat="1" ht="30">
       <c r="A74" s="5">
         <v>43608</v>
       </c>
@@ -3433,7 +3445,7 @@
         <v>20</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="1" customFormat="1">
@@ -3447,7 +3459,7 @@
         <v>6</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="1" customFormat="1">
@@ -3461,7 +3473,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3475,10 +3487,10 @@
         <v>20</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>101</v>
+        <v>138</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3492,7 +3504,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3506,7 +3518,7 @@
         <v>6</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="1" customFormat="1" ht="75">
@@ -3520,7 +3532,7 @@
         <v>6</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3534,7 +3546,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="1" customFormat="1">
@@ -3548,7 +3560,7 @@
         <v>6</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="1" customFormat="1">
@@ -3562,7 +3574,7 @@
         <v>4</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3576,7 +3588,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3590,7 +3602,7 @@
         <v>20</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3604,7 +3616,7 @@
         <v>6</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3618,7 +3630,7 @@
         <v>20</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="60">
@@ -3632,7 +3644,7 @@
         <v>20</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="1" customFormat="1">
@@ -3646,7 +3658,7 @@
         <v>20</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3660,10 +3672,10 @@
         <v>20</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3677,7 +3689,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3691,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="1" customFormat="1">
@@ -3705,7 +3717,7 @@
         <v>4</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3719,7 +3731,7 @@
         <v>5</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3733,7 +3745,7 @@
         <v>20</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="1" customFormat="1">
@@ -3747,7 +3759,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3761,7 +3773,7 @@
         <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="1" customFormat="1" ht="45">
@@ -3775,10 +3787,10 @@
         <v>20</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3792,7 +3804,7 @@
         <v>6</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3806,7 +3818,7 @@
         <v>20</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="1" customFormat="1">
@@ -3820,7 +3832,7 @@
         <v>6</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3834,7 +3846,7 @@
         <v>4</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3848,7 +3860,7 @@
         <v>5</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3862,7 +3874,7 @@
         <v>20</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="1:5" s="1" customFormat="1">
@@ -3876,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="1" customFormat="1">
@@ -3890,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="107" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3904,7 +3916,7 @@
         <v>20</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3918,7 +3930,7 @@
         <v>4</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="109" spans="1:5" s="1" customFormat="1" ht="30">
@@ -3932,63 +3944,103 @@
         <v>6</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" s="1" customFormat="1">
-      <c r="A110" s="5"/>
-      <c r="D110" s="2"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" s="1" customFormat="1" ht="60">
+      <c r="A110" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="111" spans="1:5" s="1" customFormat="1">
-      <c r="A111" s="5"/>
-      <c r="D111" s="2"/>
-    </row>
-    <row r="116" spans="8:9" ht="30">
-      <c r="H116" s="3" t="s">
+      <c r="A111" s="5">
+        <v>43620</v>
+      </c>
+      <c r="B111" s="1">
         <v>1</v>
       </c>
-      <c r="I116" s="1" t="s">
+      <c r="C111" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" s="1" customFormat="1">
+      <c r="A112" s="5"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:9" s="1" customFormat="1">
+      <c r="A113" s="5"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:9" s="1" customFormat="1">
+      <c r="A114" s="5"/>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:9" s="1" customFormat="1">
+      <c r="A115" s="5"/>
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="1:9" s="1" customFormat="1">
+      <c r="A116" s="5"/>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="121" spans="1:9" ht="30">
+      <c r="H121" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I121" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="8:9">
-      <c r="H117" s="4" t="s">
+    <row r="122" spans="1:9">
+      <c r="H122" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I117" s="2">
+      <c r="I122" s="2">
         <v>6.75</v>
       </c>
     </row>
-    <row r="118" spans="8:9">
-      <c r="H118" s="4" t="s">
+    <row r="123" spans="1:9">
+      <c r="H123" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I118" s="2">
+      <c r="I123" s="2">
         <v>24.25</v>
       </c>
     </row>
-    <row r="119" spans="8:9">
-      <c r="H119" s="4" t="s">
+    <row r="124" spans="1:9">
+      <c r="H124" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I119" s="2">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="120" spans="8:9">
-      <c r="H120" s="4" t="s">
+      <c r="I124" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="H125" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I120" s="2">
+      <c r="I125" s="2">
         <v>34.75</v>
       </c>
     </row>
-    <row r="121" spans="8:9">
-      <c r="H121" s="4" t="s">
+    <row r="126" spans="1:9">
+      <c r="H126" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I121" s="2">
-        <v>83.25</v>
+      <c r="I126" s="2">
+        <v>85.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on final docs
</commit_message>
<xml_diff>
--- a/Documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/Documentation/PHILIBERT_JournalDeBord.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="143">
   <si>
     <t>Date</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>Documentation des endpoints de l'API</t>
+  </si>
+  <si>
+    <t>Préparation du rendu final, ajout des annexes, préparation des CDs</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -998,7 +1001,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Journal!$I$121</c:f>
+              <c:f>Journal!$D$120</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1146,7 +1149,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Journal!$H$122:$H$126</c:f>
+              <c:f>Journal!$C$121:$C$125</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1166,21 +1169,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Journal!$I$122:$I$126</c:f>
+              <c:f>Journal!$D$121:$D$125</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.75</c:v>
+                  <c:v>7.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.5</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.75</c:v>
+                  <c:v>36.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1859,14 +1862,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:colOff>548527</xdr:colOff>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>459440</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:colOff>560293</xdr:colOff>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>107174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1892,7 +1895,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43621.335703703706" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="115">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PHILIBERT Alexandre" refreshedDate="43621.436421643521" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="115">
   <cacheSource type="worksheet">
     <worksheetSource name="Journal[[Date]:[Type]]"/>
   </cacheSource>
@@ -1901,7 +1904,7 @@
       <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2019-05-07T00:00:00" maxDate="2019-06-06T00:00:00"/>
     </cacheField>
     <cacheField name="Temps (h)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.25" maxValue="2.5"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -1922,8 +1925,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
-  <location ref="H121:I126" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Type">
+  <location ref="C120:D125" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -2062,14 +2065,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E116" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
-  <autoFilter ref="A1:E116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Journal" displayName="Journal" ref="A1:E113" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
+  <autoFilter ref="A1:E113"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="10"/>
     <tableColumn id="2" name="Temps (h)" dataDxfId="9"/>
     <tableColumn id="3" name="Type" dataDxfId="8"/>
-    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="7"/>
-    <tableColumn id="5" name="Retour d'expérience" dataDxfId="6"/>
+    <tableColumn id="4" name="Description" totalsRowFunction="count" dataDxfId="6"/>
+    <tableColumn id="5" name="Retour d'expérience" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2338,18 +2341,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A114" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="56.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="16.140625" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
@@ -3510,7 +3513,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="79" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A79" s="5">
         <v>43609</v>
       </c>
@@ -3594,7 +3597,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="1" customFormat="1" ht="30">
+    <row r="85" spans="1:5" s="1" customFormat="1" ht="45">
       <c r="A85" s="5">
         <v>43609</v>
       </c>
@@ -3972,7 +3975,7 @@
         <v>1</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>140</v>
@@ -3983,7 +3986,7 @@
         <v>43621</v>
       </c>
       <c r="B112" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>6</v>
@@ -3992,68 +3995,66 @@
         <v>141</v>
       </c>
     </row>
-    <row r="113" spans="1:9" s="1" customFormat="1">
-      <c r="A113" s="5"/>
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="1:9" s="1" customFormat="1">
-      <c r="A114" s="5"/>
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="1:9" s="1" customFormat="1">
-      <c r="A115" s="5"/>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="1:9" s="1" customFormat="1">
-      <c r="A116" s="5"/>
-      <c r="D116" s="2"/>
-    </row>
-    <row r="121" spans="1:9" ht="30">
-      <c r="H121" s="3" t="s">
+    <row r="113" spans="1:4" s="1" customFormat="1" ht="30">
+      <c r="A113" s="5">
+        <v>43621</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="C120" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I121" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
-      <c r="H122" s="4" t="s">
+    <row r="121" spans="1:4">
+      <c r="C121" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I122" s="2">
-        <v>6.75</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
-      <c r="H123" s="4" t="s">
+      <c r="D121" s="2">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="C122" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I123" s="2">
+      <c r="D122" s="2">
         <v>24.25</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
-      <c r="H124" s="4" t="s">
+    <row r="123" spans="1:4">
+      <c r="C123" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I124" s="2">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
-      <c r="H125" s="4" t="s">
+      <c r="D123" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="C124" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I125" s="2">
-        <v>35.75</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
-      <c r="H126" s="4" t="s">
+      <c r="D124" s="2">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="C125" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I126" s="2">
-        <v>86.25</v>
+      <c r="D125" s="2">
+        <v>89.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>